<commit_message>
updated the date_added column
</commit_message>
<xml_diff>
--- a/processed_file.xlsx
+++ b/processed_file.xlsx
@@ -685,7 +685,11 @@
       <c r="W2" t="n">
         <v>0</v>
       </c>
-      <c r="X2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>BA9333203</t>
+        </is>
+      </c>
       <c r="Y2" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -694,7 +698,7 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB2" t="n">
@@ -813,7 +817,11 @@
       <c r="W3" t="n">
         <v>-3.54</v>
       </c>
-      <c r="X3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>SA0128447</t>
+        </is>
+      </c>
       <c r="Y3" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -822,7 +830,7 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB3" t="n">
@@ -941,7 +949,11 @@
       <c r="W4" t="n">
         <v>0</v>
       </c>
-      <c r="X4" t="inlineStr"/>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>ZH608357</t>
+        </is>
+      </c>
       <c r="Y4" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -950,7 +962,7 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB4" t="n">
@@ -1069,7 +1081,11 @@
       <c r="W5" t="n">
         <v>0</v>
       </c>
-      <c r="X5" t="inlineStr"/>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>BA9329460</t>
+        </is>
+      </c>
       <c r="Y5" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1078,7 +1094,7 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB5" t="n">
@@ -1197,7 +1213,11 @@
       <c r="W6" t="n">
         <v>0</v>
       </c>
-      <c r="X6" t="inlineStr"/>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>BA9327309</t>
+        </is>
+      </c>
       <c r="Y6" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1206,7 +1226,7 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB6" t="n">
@@ -1325,7 +1345,11 @@
       <c r="W7" t="n">
         <v>0</v>
       </c>
-      <c r="X7" t="inlineStr"/>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>BA9327716</t>
+        </is>
+      </c>
       <c r="Y7" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1334,7 +1358,7 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB7" t="n">
@@ -1453,7 +1477,11 @@
       <c r="W8" t="n">
         <v>0</v>
       </c>
-      <c r="X8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>K615670</t>
+        </is>
+      </c>
       <c r="Y8" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1462,7 +1490,7 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB8" t="n">
@@ -1581,7 +1609,11 @@
       <c r="W9" t="n">
         <v>0</v>
       </c>
-      <c r="X9" t="inlineStr"/>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>AB0086694</t>
+        </is>
+      </c>
       <c r="Y9" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1590,7 +1622,7 @@
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB9" t="n">
@@ -1709,7 +1741,11 @@
       <c r="W10" t="n">
         <v>-39</v>
       </c>
-      <c r="X10" t="inlineStr"/>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>SA0129343</t>
+        </is>
+      </c>
       <c r="Y10" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1718,7 +1754,7 @@
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB10" t="n">
@@ -1837,7 +1873,11 @@
       <c r="W11" t="n">
         <v>0</v>
       </c>
-      <c r="X11" t="inlineStr"/>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>ZH596674</t>
+        </is>
+      </c>
       <c r="Y11" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1846,7 +1886,7 @@
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB11" t="n">
@@ -1965,7 +2005,11 @@
       <c r="W12" t="n">
         <v>0</v>
       </c>
-      <c r="X12" t="inlineStr"/>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>BA9318113</t>
+        </is>
+      </c>
       <c r="Y12" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -1974,7 +2018,7 @@
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB12" t="n">
@@ -2089,7 +2133,11 @@
       <c r="W13" t="n">
         <v>0</v>
       </c>
-      <c r="X13" t="inlineStr"/>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>BA9318238</t>
+        </is>
+      </c>
       <c r="Y13" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2098,7 +2146,7 @@
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB13" t="n">
@@ -2217,7 +2265,11 @@
       <c r="W14" t="n">
         <v>0</v>
       </c>
-      <c r="X14" t="inlineStr"/>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>BA9321727</t>
+        </is>
+      </c>
       <c r="Y14" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2226,7 +2278,7 @@
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB14" t="n">
@@ -2345,7 +2397,11 @@
       <c r="W15" t="n">
         <v>0</v>
       </c>
-      <c r="X15" t="inlineStr"/>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>BA9315438</t>
+        </is>
+      </c>
       <c r="Y15" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2354,7 +2410,7 @@
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB15" t="n">
@@ -2473,7 +2529,11 @@
       <c r="W16" t="n">
         <v>0</v>
       </c>
-      <c r="X16" t="inlineStr"/>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>K614825</t>
+        </is>
+      </c>
       <c r="Y16" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2482,7 +2542,7 @@
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB16" t="n">
@@ -2597,7 +2657,11 @@
       <c r="W17" t="n">
         <v>0</v>
       </c>
-      <c r="X17" t="inlineStr"/>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>AA9968051</t>
+        </is>
+      </c>
       <c r="Y17" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2606,7 +2670,7 @@
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB17" t="n">
@@ -2725,7 +2789,11 @@
       <c r="W18" t="n">
         <v>0</v>
       </c>
-      <c r="X18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>223150301111347</t>
+        </is>
+      </c>
       <c r="Y18" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2734,7 +2802,7 @@
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB18" t="n">
@@ -2853,7 +2921,11 @@
       <c r="W19" t="n">
         <v>0</v>
       </c>
-      <c r="X19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>113150306487493</t>
+        </is>
+      </c>
       <c r="Y19" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2862,7 +2934,7 @@
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB19" t="n">
@@ -2981,7 +3053,11 @@
       <c r="W20" t="n">
         <v>-39</v>
       </c>
-      <c r="X20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>SA0128943</t>
+        </is>
+      </c>
       <c r="Y20" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -2990,7 +3066,7 @@
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB20" t="n">
@@ -3109,7 +3185,11 @@
       <c r="W21" t="n">
         <v>0</v>
       </c>
-      <c r="X21" t="inlineStr"/>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>BA9308002</t>
+        </is>
+      </c>
       <c r="Y21" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3118,7 +3198,7 @@
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB21" t="n">
@@ -3237,7 +3317,11 @@
       <c r="W22" t="n">
         <v>0</v>
       </c>
-      <c r="X22" t="inlineStr"/>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>AA9945857</t>
+        </is>
+      </c>
       <c r="Y22" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3246,7 +3330,7 @@
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB22" t="n">
@@ -3365,7 +3449,11 @@
       <c r="W23" t="n">
         <v>0</v>
       </c>
-      <c r="X23" t="inlineStr"/>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>AA9941224</t>
+        </is>
+      </c>
       <c r="Y23" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3374,7 +3462,7 @@
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB23" t="n">
@@ -3493,7 +3581,11 @@
       <c r="W24" t="n">
         <v>0</v>
       </c>
-      <c r="X24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>AA9931265</t>
+        </is>
+      </c>
       <c r="Y24" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3502,7 +3594,7 @@
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB24" t="n">
@@ -3621,7 +3713,11 @@
       <c r="W25" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X25" t="inlineStr"/>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>ZH575711</t>
+        </is>
+      </c>
       <c r="Y25" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3630,7 +3726,7 @@
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB25" t="n">
@@ -3749,7 +3845,11 @@
       <c r="W26" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X26" t="inlineStr"/>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>ZH575941</t>
+        </is>
+      </c>
       <c r="Y26" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3758,7 +3858,7 @@
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB26" t="n">
@@ -3877,7 +3977,11 @@
       <c r="W27" t="n">
         <v>0</v>
       </c>
-      <c r="X27" t="inlineStr"/>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>BA9294434</t>
+        </is>
+      </c>
       <c r="Y27" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -3886,7 +3990,7 @@
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB27" t="n">
@@ -4005,7 +4109,11 @@
       <c r="W28" t="n">
         <v>0</v>
       </c>
-      <c r="X28" t="inlineStr"/>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>AA9887842</t>
+        </is>
+      </c>
       <c r="Y28" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4014,7 +4122,7 @@
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB28" t="n">
@@ -4133,7 +4241,11 @@
       <c r="W29" t="n">
         <v>0</v>
       </c>
-      <c r="X29" t="inlineStr"/>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>AA9918832</t>
+        </is>
+      </c>
       <c r="Y29" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4142,7 +4254,7 @@
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB29" t="n">
@@ -4261,7 +4373,11 @@
       <c r="W30" t="n">
         <v>0</v>
       </c>
-      <c r="X30" t="inlineStr"/>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>ZD675769</t>
+        </is>
+      </c>
       <c r="Y30" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4270,7 +4386,7 @@
       <c r="Z30" t="inlineStr"/>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB30" t="n">
@@ -4389,7 +4505,11 @@
       <c r="W31" t="n">
         <v>0</v>
       </c>
-      <c r="X31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>J194275</t>
+        </is>
+      </c>
       <c r="Y31" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4398,7 +4518,7 @@
       <c r="Z31" t="inlineStr"/>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB31" t="n">
@@ -4517,7 +4637,11 @@
       <c r="W32" t="n">
         <v>0</v>
       </c>
-      <c r="X32" t="inlineStr"/>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>AA9854593</t>
+        </is>
+      </c>
       <c r="Y32" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4526,7 +4650,7 @@
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB32" t="n">
@@ -4645,7 +4769,11 @@
       <c r="W33" t="n">
         <v>0</v>
       </c>
-      <c r="X33" t="inlineStr"/>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>BA9288651</t>
+        </is>
+      </c>
       <c r="Y33" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4654,7 +4782,7 @@
       <c r="Z33" t="inlineStr"/>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB33" t="n">
@@ -4773,7 +4901,11 @@
       <c r="W34" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X34" t="inlineStr"/>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>AA9863979</t>
+        </is>
+      </c>
       <c r="Y34" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4782,7 +4914,7 @@
       <c r="Z34" t="inlineStr"/>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB34" t="n">
@@ -4901,7 +5033,11 @@
       <c r="W35" t="n">
         <v>0</v>
       </c>
-      <c r="X35" t="inlineStr"/>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>AA9842553</t>
+        </is>
+      </c>
       <c r="Y35" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -4910,7 +5046,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB35" t="n">
@@ -5029,7 +5165,11 @@
       <c r="W36" t="n">
         <v>0</v>
       </c>
-      <c r="X36" t="inlineStr"/>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>AA9841628</t>
+        </is>
+      </c>
       <c r="Y36" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5038,7 +5178,7 @@
       <c r="Z36" t="inlineStr"/>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB36" t="n">
@@ -5157,7 +5297,11 @@
       <c r="W37" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X37" t="inlineStr"/>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>AA9823298</t>
+        </is>
+      </c>
       <c r="Y37" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5166,7 +5310,7 @@
       <c r="Z37" t="inlineStr"/>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB37" t="n">
@@ -5285,7 +5429,11 @@
       <c r="W38" t="n">
         <v>0</v>
       </c>
-      <c r="X38" t="inlineStr"/>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>113150306477958</t>
+        </is>
+      </c>
       <c r="Y38" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5294,7 +5442,7 @@
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB38" t="n">
@@ -5413,7 +5561,11 @@
       <c r="W39" t="n">
         <v>0</v>
       </c>
-      <c r="X39" t="inlineStr"/>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>113150306477958</t>
+        </is>
+      </c>
       <c r="Y39" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5422,7 +5574,7 @@
       <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB39" t="n">
@@ -5541,7 +5693,11 @@
       <c r="W40" t="n">
         <v>-12.45</v>
       </c>
-      <c r="X40" t="inlineStr"/>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>ZH561112</t>
+        </is>
+      </c>
       <c r="Y40" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5550,7 +5706,7 @@
       <c r="Z40" t="inlineStr"/>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB40" t="n">
@@ -5669,7 +5825,11 @@
       <c r="W41" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="X41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>ZH560906</t>
+        </is>
+      </c>
       <c r="Y41" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5678,7 +5838,7 @@
       <c r="Z41" t="inlineStr"/>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB41" t="n">
@@ -5797,7 +5957,11 @@
       <c r="W42" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="X42" t="inlineStr"/>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>ZH560906</t>
+        </is>
+      </c>
       <c r="Y42" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5806,7 +5970,7 @@
       <c r="Z42" t="inlineStr"/>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB42" t="n">
@@ -5925,7 +6089,11 @@
       <c r="W43" t="n">
         <v>0</v>
       </c>
-      <c r="X43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>BA9281454</t>
+        </is>
+      </c>
       <c r="Y43" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -5934,7 +6102,7 @@
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB43" t="n">
@@ -6053,7 +6221,11 @@
       <c r="W44" t="n">
         <v>0</v>
       </c>
-      <c r="X44" t="inlineStr"/>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>BA9280947</t>
+        </is>
+      </c>
       <c r="Y44" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6062,7 +6234,7 @@
       <c r="Z44" t="inlineStr"/>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB44" t="n">
@@ -6177,7 +6349,11 @@
       <c r="W45" t="n">
         <v>0</v>
       </c>
-      <c r="X45" t="inlineStr"/>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>AA9809417</t>
+        </is>
+      </c>
       <c r="Y45" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6186,7 +6362,7 @@
       <c r="Z45" t="inlineStr"/>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB45" t="n">
@@ -6305,7 +6481,11 @@
       <c r="W46" t="n">
         <v>0</v>
       </c>
-      <c r="X46" t="inlineStr"/>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>BA9277531</t>
+        </is>
+      </c>
       <c r="Y46" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6314,7 +6494,7 @@
       <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB46" t="n">
@@ -6433,7 +6613,11 @@
       <c r="W47" t="n">
         <v>0</v>
       </c>
-      <c r="X47" t="inlineStr"/>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>BA9277531</t>
+        </is>
+      </c>
       <c r="Y47" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6442,7 +6626,7 @@
       <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB47" t="n">
@@ -6561,7 +6745,11 @@
       <c r="W48" t="n">
         <v>0</v>
       </c>
-      <c r="X48" t="inlineStr"/>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>BA9277531</t>
+        </is>
+      </c>
       <c r="Y48" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6570,7 +6758,7 @@
       <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB48" t="n">
@@ -6685,7 +6873,11 @@
       <c r="W49" t="n">
         <v>0</v>
       </c>
-      <c r="X49" t="inlineStr"/>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>BA9276559</t>
+        </is>
+      </c>
       <c r="Y49" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6694,7 +6886,7 @@
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB49" t="n">
@@ -6809,7 +7001,11 @@
       <c r="W50" t="n">
         <v>0</v>
       </c>
-      <c r="X50" t="inlineStr"/>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>AA9793409</t>
+        </is>
+      </c>
       <c r="Y50" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6818,7 +7014,7 @@
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB50" t="n">
@@ -6937,7 +7133,11 @@
       <c r="W51" t="n">
         <v>0</v>
       </c>
-      <c r="X51" t="inlineStr"/>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>BA9279274</t>
+        </is>
+      </c>
       <c r="Y51" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -6946,7 +7146,7 @@
       <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB51" t="n">
@@ -7065,7 +7265,11 @@
       <c r="W52" t="n">
         <v>0</v>
       </c>
-      <c r="X52" t="inlineStr"/>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>AA9774405</t>
+        </is>
+      </c>
       <c r="Y52" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7074,7 +7278,7 @@
       <c r="Z52" t="inlineStr"/>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB52" t="n">
@@ -7189,7 +7393,11 @@
       <c r="W53" t="n">
         <v>0</v>
       </c>
-      <c r="X53" t="inlineStr"/>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>AA9769276</t>
+        </is>
+      </c>
       <c r="Y53" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7198,7 +7406,7 @@
       <c r="Z53" t="inlineStr"/>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB53" t="n">
@@ -7313,7 +7521,11 @@
       <c r="W54" t="n">
         <v>0</v>
       </c>
-      <c r="X54" t="inlineStr"/>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>AA9768963</t>
+        </is>
+      </c>
       <c r="Y54" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7322,7 +7534,7 @@
       <c r="Z54" t="inlineStr"/>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB54" t="n">
@@ -7441,7 +7653,11 @@
       <c r="W55" t="n">
         <v>0</v>
       </c>
-      <c r="X55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>AA9770354</t>
+        </is>
+      </c>
       <c r="Y55" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7450,7 +7666,7 @@
       <c r="Z55" t="inlineStr"/>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB55" t="n">
@@ -7565,7 +7781,11 @@
       <c r="W56" t="n">
         <v>0</v>
       </c>
-      <c r="X56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>AA9771929</t>
+        </is>
+      </c>
       <c r="Y56" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7574,7 +7794,7 @@
       <c r="Z56" t="inlineStr"/>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB56" t="n">
@@ -7693,7 +7913,11 @@
       <c r="W57" t="n">
         <v>0</v>
       </c>
-      <c r="X57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>AA9781655</t>
+        </is>
+      </c>
       <c r="Y57" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7702,7 +7926,7 @@
       <c r="Z57" t="inlineStr"/>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB57" t="n">
@@ -7821,7 +8045,11 @@
       <c r="W58" t="n">
         <v>0</v>
       </c>
-      <c r="X58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>113150306474491</t>
+        </is>
+      </c>
       <c r="Y58" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7830,7 +8058,7 @@
       <c r="Z58" t="inlineStr"/>
       <c r="AA58" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB58" t="n">
@@ -7949,7 +8177,11 @@
       <c r="W59" t="n">
         <v>0</v>
       </c>
-      <c r="X59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>ZH545836</t>
+        </is>
+      </c>
       <c r="Y59" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -7958,7 +8190,7 @@
       <c r="Z59" t="inlineStr"/>
       <c r="AA59" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB59" t="n">
@@ -8077,7 +8309,11 @@
       <c r="W60" t="n">
         <v>0</v>
       </c>
-      <c r="X60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>ZD673405</t>
+        </is>
+      </c>
       <c r="Y60" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8086,7 +8322,7 @@
       <c r="Z60" t="inlineStr"/>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB60" t="n">
@@ -8205,7 +8441,11 @@
       <c r="W61" t="n">
         <v>0</v>
       </c>
-      <c r="X61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>BA9268636</t>
+        </is>
+      </c>
       <c r="Y61" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8214,7 +8454,7 @@
       <c r="Z61" t="inlineStr"/>
       <c r="AA61" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB61" t="n">
@@ -8333,7 +8573,11 @@
       <c r="W62" t="n">
         <v>0</v>
       </c>
-      <c r="X62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>BA9269864</t>
+        </is>
+      </c>
       <c r="Y62" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8342,7 +8586,7 @@
       <c r="Z62" t="inlineStr"/>
       <c r="AA62" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB62" t="n">
@@ -8461,7 +8705,11 @@
       <c r="W63" t="n">
         <v>0</v>
       </c>
-      <c r="X63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>AA9720616</t>
+        </is>
+      </c>
       <c r="Y63" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8470,7 +8718,7 @@
       <c r="Z63" t="inlineStr"/>
       <c r="AA63" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB63" t="n">
@@ -8589,7 +8837,11 @@
       <c r="W64" t="n">
         <v>0</v>
       </c>
-      <c r="X64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>BA9269831</t>
+        </is>
+      </c>
       <c r="Y64" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8598,7 +8850,7 @@
       <c r="Z64" t="inlineStr"/>
       <c r="AA64" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB64" t="n">
@@ -8717,7 +8969,11 @@
       <c r="W65" t="n">
         <v>0</v>
       </c>
-      <c r="X65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>BA9261727</t>
+        </is>
+      </c>
       <c r="Y65" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8726,7 +8982,7 @@
       <c r="Z65" t="inlineStr"/>
       <c r="AA65" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB65" t="n">
@@ -8845,7 +9101,11 @@
       <c r="W66" t="n">
         <v>0</v>
       </c>
-      <c r="X66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>BA9261727</t>
+        </is>
+      </c>
       <c r="Y66" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8854,7 +9114,7 @@
       <c r="Z66" t="inlineStr"/>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB66" t="n">
@@ -8969,7 +9229,11 @@
       <c r="W67" t="n">
         <v>0</v>
       </c>
-      <c r="X67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>BA9265979</t>
+        </is>
+      </c>
       <c r="Y67" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -8978,7 +9242,7 @@
       <c r="Z67" t="inlineStr"/>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB67" t="n">
@@ -9097,7 +9361,11 @@
       <c r="W68" t="n">
         <v>0</v>
       </c>
-      <c r="X68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>BA9266139</t>
+        </is>
+      </c>
       <c r="Y68" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9106,7 +9374,7 @@
       <c r="Z68" t="inlineStr"/>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB68" t="n">
@@ -9225,7 +9493,11 @@
       <c r="W69" t="n">
         <v>0</v>
       </c>
-      <c r="X69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>BA9267013</t>
+        </is>
+      </c>
       <c r="Y69" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9234,7 +9506,7 @@
       <c r="Z69" t="inlineStr"/>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB69" t="n">
@@ -9353,7 +9625,11 @@
       <c r="W70" t="n">
         <v>0</v>
       </c>
-      <c r="X70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>AA9722986</t>
+        </is>
+      </c>
       <c r="Y70" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9362,7 +9638,7 @@
       <c r="Z70" t="inlineStr"/>
       <c r="AA70" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB70" t="n">
@@ -9481,7 +9757,11 @@
       <c r="W71" t="n">
         <v>0</v>
       </c>
-      <c r="X71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>AA9722986</t>
+        </is>
+      </c>
       <c r="Y71" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9490,7 +9770,7 @@
       <c r="Z71" t="inlineStr"/>
       <c r="AA71" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB71" t="n">
@@ -9605,7 +9885,11 @@
       <c r="W72" t="n">
         <v>0</v>
       </c>
-      <c r="X72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>AA9754451</t>
+        </is>
+      </c>
       <c r="Y72" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9614,7 +9898,7 @@
       <c r="Z72" t="inlineStr"/>
       <c r="AA72" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB72" t="n">
@@ -9733,7 +10017,11 @@
       <c r="W73" t="n">
         <v>0</v>
       </c>
-      <c r="X73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>AA9744305</t>
+        </is>
+      </c>
       <c r="Y73" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9742,7 +10030,7 @@
       <c r="Z73" t="inlineStr"/>
       <c r="AA73" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB73" t="n">
@@ -9861,7 +10149,11 @@
       <c r="W74" t="n">
         <v>0</v>
       </c>
-      <c r="X74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>AA9732211</t>
+        </is>
+      </c>
       <c r="Y74" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9870,7 +10162,7 @@
       <c r="Z74" t="inlineStr"/>
       <c r="AA74" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB74" t="n">
@@ -9985,7 +10277,11 @@
       <c r="W75" t="n">
         <v>0</v>
       </c>
-      <c r="X75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>AA9721534</t>
+        </is>
+      </c>
       <c r="Y75" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -9994,7 +10290,7 @@
       <c r="Z75" t="inlineStr"/>
       <c r="AA75" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB75" t="n">
@@ -10113,7 +10409,11 @@
       <c r="W76" t="n">
         <v>0</v>
       </c>
-      <c r="X76" t="inlineStr"/>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>AA9737743</t>
+        </is>
+      </c>
       <c r="Y76" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10122,7 +10422,7 @@
       <c r="Z76" t="inlineStr"/>
       <c r="AA76" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB76" t="n">
@@ -10241,7 +10541,11 @@
       <c r="W77" t="n">
         <v>0</v>
       </c>
-      <c r="X77" t="inlineStr"/>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>ZH542120</t>
+        </is>
+      </c>
       <c r="Y77" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10250,7 +10554,7 @@
       <c r="Z77" t="inlineStr"/>
       <c r="AA77" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB77" t="n">
@@ -10369,7 +10673,11 @@
       <c r="W78" t="n">
         <v>0</v>
       </c>
-      <c r="X78" t="inlineStr"/>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>AA9723022</t>
+        </is>
+      </c>
       <c r="Y78" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10378,7 +10686,7 @@
       <c r="Z78" t="inlineStr"/>
       <c r="AA78" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB78" t="n">
@@ -10497,7 +10805,11 @@
       <c r="W79" t="n">
         <v>0</v>
       </c>
-      <c r="X79" t="inlineStr"/>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>AA9720348</t>
+        </is>
+      </c>
       <c r="Y79" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10506,7 +10818,7 @@
       <c r="Z79" t="inlineStr"/>
       <c r="AA79" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB79" t="n">
@@ -10625,7 +10937,11 @@
       <c r="W80" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="X80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>AA9732530</t>
+        </is>
+      </c>
       <c r="Y80" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10634,7 +10950,7 @@
       <c r="Z80" t="inlineStr"/>
       <c r="AA80" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB80" t="n">
@@ -10753,7 +11069,11 @@
       <c r="W81" t="n">
         <v>-39</v>
       </c>
-      <c r="X81" t="inlineStr"/>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>SA0126629</t>
+        </is>
+      </c>
       <c r="Y81" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10762,7 +11082,7 @@
       <c r="Z81" t="inlineStr"/>
       <c r="AA81" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB81" t="n">
@@ -10877,7 +11197,11 @@
       <c r="W82" t="n">
         <v>0</v>
       </c>
-      <c r="X82" t="inlineStr"/>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>113150306469246</t>
+        </is>
+      </c>
       <c r="Y82" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -10886,7 +11210,7 @@
       <c r="Z82" t="inlineStr"/>
       <c r="AA82" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB82" t="n">
@@ -11005,7 +11329,11 @@
       <c r="W83" t="n">
         <v>0</v>
       </c>
-      <c r="X83" t="inlineStr"/>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>113150306469930</t>
+        </is>
+      </c>
       <c r="Y83" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11014,7 +11342,7 @@
       <c r="Z83" t="inlineStr"/>
       <c r="AA83" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB83" t="n">
@@ -11133,7 +11461,11 @@
       <c r="W84" t="n">
         <v>0</v>
       </c>
-      <c r="X84" t="inlineStr"/>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>ZD670845</t>
+        </is>
+      </c>
       <c r="Y84" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11142,7 +11474,7 @@
       <c r="Z84" t="inlineStr"/>
       <c r="AA84" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB84" t="n">
@@ -11261,7 +11593,11 @@
       <c r="W85" t="n">
         <v>0</v>
       </c>
-      <c r="X85" t="inlineStr"/>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>BA9252349</t>
+        </is>
+      </c>
       <c r="Y85" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11270,7 +11606,7 @@
       <c r="Z85" t="inlineStr"/>
       <c r="AA85" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB85" t="n">
@@ -11385,7 +11721,11 @@
       <c r="W86" t="n">
         <v>0</v>
       </c>
-      <c r="X86" t="inlineStr"/>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>BA9247061</t>
+        </is>
+      </c>
       <c r="Y86" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11394,7 +11734,7 @@
       <c r="Z86" t="inlineStr"/>
       <c r="AA86" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB86" t="n">
@@ -11513,7 +11853,11 @@
       <c r="W87" t="n">
         <v>0</v>
       </c>
-      <c r="X87" t="inlineStr"/>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>AA9700042</t>
+        </is>
+      </c>
       <c r="Y87" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11522,7 +11866,7 @@
       <c r="Z87" t="inlineStr"/>
       <c r="AA87" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB87" t="n">
@@ -11637,7 +11981,11 @@
       <c r="W88" t="n">
         <v>0</v>
       </c>
-      <c r="X88" t="inlineStr"/>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>BA9256207</t>
+        </is>
+      </c>
       <c r="Y88" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11646,7 +11994,7 @@
       <c r="Z88" t="inlineStr"/>
       <c r="AA88" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB88" t="n">
@@ -11765,7 +12113,11 @@
       <c r="W89" t="n">
         <v>0</v>
       </c>
-      <c r="X89" t="inlineStr"/>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>BA9253725</t>
+        </is>
+      </c>
       <c r="Y89" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11774,7 +12126,7 @@
       <c r="Z89" t="inlineStr"/>
       <c r="AA89" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB89" t="n">
@@ -11889,7 +12241,11 @@
       <c r="W90" t="n">
         <v>0</v>
       </c>
-      <c r="X90" t="inlineStr"/>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>BA9252342</t>
+        </is>
+      </c>
       <c r="Y90" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -11898,7 +12254,7 @@
       <c r="Z90" t="inlineStr"/>
       <c r="AA90" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB90" t="n">
@@ -12017,7 +12373,11 @@
       <c r="W91" t="n">
         <v>0</v>
       </c>
-      <c r="X91" t="inlineStr"/>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>BA9254221</t>
+        </is>
+      </c>
       <c r="Y91" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12026,7 +12386,7 @@
       <c r="Z91" t="inlineStr"/>
       <c r="AA91" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB91" t="n">
@@ -12141,7 +12501,11 @@
       <c r="W92" t="n">
         <v>0</v>
       </c>
-      <c r="X92" t="inlineStr"/>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>BA9253777</t>
+        </is>
+      </c>
       <c r="Y92" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12150,7 +12514,7 @@
       <c r="Z92" t="inlineStr"/>
       <c r="AA92" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB92" t="n">
@@ -12265,7 +12629,11 @@
       <c r="W93" t="n">
         <v>0</v>
       </c>
-      <c r="X93" t="inlineStr"/>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>BA9253777</t>
+        </is>
+      </c>
       <c r="Y93" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12274,7 +12642,7 @@
       <c r="Z93" t="inlineStr"/>
       <c r="AA93" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB93" t="n">
@@ -12393,7 +12761,11 @@
       <c r="W94" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X94" t="inlineStr"/>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>AA9703828</t>
+        </is>
+      </c>
       <c r="Y94" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12402,7 +12774,7 @@
       <c r="Z94" t="inlineStr"/>
       <c r="AA94" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB94" t="n">
@@ -12521,7 +12893,11 @@
       <c r="W95" t="n">
         <v>0</v>
       </c>
-      <c r="X95" t="inlineStr"/>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>BA9250599</t>
+        </is>
+      </c>
       <c r="Y95" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12530,7 +12906,7 @@
       <c r="Z95" t="inlineStr"/>
       <c r="AA95" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB95" t="n">
@@ -12649,7 +13025,11 @@
       <c r="W96" t="n">
         <v>0</v>
       </c>
-      <c r="X96" t="inlineStr"/>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>BA9254907</t>
+        </is>
+      </c>
       <c r="Y96" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12658,7 +13038,7 @@
       <c r="Z96" t="inlineStr"/>
       <c r="AA96" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB96" t="n">
@@ -12777,7 +13157,11 @@
       <c r="W97" t="n">
         <v>-12.45</v>
       </c>
-      <c r="X97" t="inlineStr"/>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>AA9699657</t>
+        </is>
+      </c>
       <c r="Y97" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12786,7 +13170,7 @@
       <c r="Z97" t="inlineStr"/>
       <c r="AA97" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB97" t="n">
@@ -12905,7 +13289,11 @@
       <c r="W98" t="n">
         <v>0</v>
       </c>
-      <c r="X98" t="inlineStr"/>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>AA9697284</t>
+        </is>
+      </c>
       <c r="Y98" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -12914,7 +13302,7 @@
       <c r="Z98" t="inlineStr"/>
       <c r="AA98" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB98" t="n">
@@ -13033,7 +13421,11 @@
       <c r="W99" t="n">
         <v>0</v>
       </c>
-      <c r="X99" t="inlineStr"/>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>AA9706500</t>
+        </is>
+      </c>
       <c r="Y99" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13042,7 +13434,7 @@
       <c r="Z99" t="inlineStr"/>
       <c r="AA99" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB99" t="n">
@@ -13161,7 +13553,11 @@
       <c r="W100" t="n">
         <v>0</v>
       </c>
-      <c r="X100" t="inlineStr"/>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>AA9689088</t>
+        </is>
+      </c>
       <c r="Y100" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13170,7 +13566,7 @@
       <c r="Z100" t="inlineStr"/>
       <c r="AA100" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB100" t="n">
@@ -13289,7 +13685,11 @@
       <c r="W101" t="n">
         <v>0</v>
       </c>
-      <c r="X101" t="inlineStr"/>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>AA9671233</t>
+        </is>
+      </c>
       <c r="Y101" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13298,7 +13698,7 @@
       <c r="Z101" t="inlineStr"/>
       <c r="AA101" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB101" t="n">
@@ -13417,7 +13817,11 @@
       <c r="W102" t="n">
         <v>0</v>
       </c>
-      <c r="X102" t="inlineStr"/>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>AA9671233</t>
+        </is>
+      </c>
       <c r="Y102" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13426,7 +13830,7 @@
       <c r="Z102" t="inlineStr"/>
       <c r="AA102" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB102" t="n">
@@ -13545,7 +13949,11 @@
       <c r="W103" t="n">
         <v>0</v>
       </c>
-      <c r="X103" t="inlineStr"/>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>BA9246178</t>
+        </is>
+      </c>
       <c r="Y103" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13554,7 +13962,7 @@
       <c r="Z103" t="inlineStr"/>
       <c r="AA103" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB103" t="n">
@@ -13673,7 +14081,11 @@
       <c r="W104" t="n">
         <v>0</v>
       </c>
-      <c r="X104" t="inlineStr"/>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>AA9653563</t>
+        </is>
+      </c>
       <c r="Y104" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13682,7 +14094,7 @@
       <c r="Z104" t="inlineStr"/>
       <c r="AA104" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB104" t="n">
@@ -13801,7 +14213,11 @@
       <c r="W105" t="n">
         <v>0</v>
       </c>
-      <c r="X105" t="inlineStr"/>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>AA9653563</t>
+        </is>
+      </c>
       <c r="Y105" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13810,7 +14226,7 @@
       <c r="Z105" t="inlineStr"/>
       <c r="AA105" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB105" t="n">
@@ -13929,7 +14345,11 @@
       <c r="W106" t="n">
         <v>0</v>
       </c>
-      <c r="X106" t="inlineStr"/>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>BA9245680</t>
+        </is>
+      </c>
       <c r="Y106" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -13938,7 +14358,7 @@
       <c r="Z106" t="inlineStr"/>
       <c r="AA106" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB106" t="n">
@@ -14057,7 +14477,11 @@
       <c r="W107" t="n">
         <v>0</v>
       </c>
-      <c r="X107" t="inlineStr"/>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>AA9661659</t>
+        </is>
+      </c>
       <c r="Y107" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14066,7 +14490,7 @@
       <c r="Z107" t="inlineStr"/>
       <c r="AA107" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB107" t="n">
@@ -14185,7 +14609,11 @@
       <c r="W108" t="n">
         <v>0</v>
       </c>
-      <c r="X108" t="inlineStr"/>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>J172997</t>
+        </is>
+      </c>
       <c r="Y108" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14194,7 +14622,7 @@
       <c r="Z108" t="inlineStr"/>
       <c r="AA108" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB108" t="n">
@@ -14313,7 +14741,11 @@
       <c r="W109" t="n">
         <v>0</v>
       </c>
-      <c r="X109" t="inlineStr"/>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>J174440</t>
+        </is>
+      </c>
       <c r="Y109" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14322,7 +14754,7 @@
       <c r="Z109" t="inlineStr"/>
       <c r="AA109" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB109" t="n">
@@ -14437,7 +14869,11 @@
       <c r="W110" t="n">
         <v>0</v>
       </c>
-      <c r="X110" t="inlineStr"/>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>AA9661244</t>
+        </is>
+      </c>
       <c r="Y110" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14446,7 +14882,7 @@
       <c r="Z110" t="inlineStr"/>
       <c r="AA110" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB110" t="n">
@@ -14565,7 +15001,11 @@
       <c r="W111" t="n">
         <v>0</v>
       </c>
-      <c r="X111" t="inlineStr"/>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t>AA9682217</t>
+        </is>
+      </c>
       <c r="Y111" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14574,7 +15014,7 @@
       <c r="Z111" t="inlineStr"/>
       <c r="AA111" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB111" t="n">
@@ -14693,7 +15133,11 @@
       <c r="W112" t="n">
         <v>0</v>
       </c>
-      <c r="X112" t="inlineStr"/>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>223150301110117</t>
+        </is>
+      </c>
       <c r="Y112" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14702,7 +15146,7 @@
       <c r="Z112" t="inlineStr"/>
       <c r="AA112" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB112" t="n">
@@ -14821,7 +15265,11 @@
       <c r="W113" t="n">
         <v>0</v>
       </c>
-      <c r="X113" t="inlineStr"/>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>J155597</t>
+        </is>
+      </c>
       <c r="Y113" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14830,7 +15278,7 @@
       <c r="Z113" t="inlineStr"/>
       <c r="AA113" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB113" t="n">
@@ -14949,7 +15397,11 @@
       <c r="W114" t="n">
         <v>0</v>
       </c>
-      <c r="X114" t="inlineStr"/>
+      <c r="X114" t="inlineStr">
+        <is>
+          <t>BA9236161</t>
+        </is>
+      </c>
       <c r="Y114" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -14958,7 +15410,7 @@
       <c r="Z114" t="inlineStr"/>
       <c r="AA114" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB114" t="n">
@@ -15077,7 +15529,11 @@
       <c r="W115" t="n">
         <v>0</v>
       </c>
-      <c r="X115" t="inlineStr"/>
+      <c r="X115" t="inlineStr">
+        <is>
+          <t>BA9228205</t>
+        </is>
+      </c>
       <c r="Y115" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15086,7 +15542,7 @@
       <c r="Z115" t="inlineStr"/>
       <c r="AA115" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB115" t="n">
@@ -15201,7 +15657,11 @@
       <c r="W116" t="n">
         <v>0</v>
       </c>
-      <c r="X116" t="inlineStr"/>
+      <c r="X116" t="inlineStr">
+        <is>
+          <t>AA9639068</t>
+        </is>
+      </c>
       <c r="Y116" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15210,7 +15670,7 @@
       <c r="Z116" t="inlineStr"/>
       <c r="AA116" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB116" t="n">
@@ -15329,7 +15789,11 @@
       <c r="W117" t="n">
         <v>0</v>
       </c>
-      <c r="X117" t="inlineStr"/>
+      <c r="X117" t="inlineStr">
+        <is>
+          <t>AA9607568</t>
+        </is>
+      </c>
       <c r="Y117" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15338,7 +15802,7 @@
       <c r="Z117" t="inlineStr"/>
       <c r="AA117" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB117" t="n">
@@ -15457,7 +15921,11 @@
       <c r="W118" t="n">
         <v>0</v>
       </c>
-      <c r="X118" t="inlineStr"/>
+      <c r="X118" t="inlineStr">
+        <is>
+          <t>BA9229187</t>
+        </is>
+      </c>
       <c r="Y118" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15466,7 +15934,7 @@
       <c r="Z118" t="inlineStr"/>
       <c r="AA118" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB118" t="n">
@@ -15585,7 +16053,11 @@
       <c r="W119" t="n">
         <v>0</v>
       </c>
-      <c r="X119" t="inlineStr"/>
+      <c r="X119" t="inlineStr">
+        <is>
+          <t>BA9228486</t>
+        </is>
+      </c>
       <c r="Y119" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15594,7 +16066,7 @@
       <c r="Z119" t="inlineStr"/>
       <c r="AA119" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB119" t="n">
@@ -15713,7 +16185,11 @@
       <c r="W120" t="n">
         <v>0</v>
       </c>
-      <c r="X120" t="inlineStr"/>
+      <c r="X120" t="inlineStr">
+        <is>
+          <t>BA9229412</t>
+        </is>
+      </c>
       <c r="Y120" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15722,7 +16198,7 @@
       <c r="Z120" t="inlineStr"/>
       <c r="AA120" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB120" t="n">
@@ -15841,7 +16317,11 @@
       <c r="W121" t="n">
         <v>0</v>
       </c>
-      <c r="X121" t="inlineStr"/>
+      <c r="X121" t="inlineStr">
+        <is>
+          <t>BA9230214</t>
+        </is>
+      </c>
       <c r="Y121" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15850,7 +16330,7 @@
       <c r="Z121" t="inlineStr"/>
       <c r="AA121" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB121" t="n">
@@ -15969,7 +16449,11 @@
       <c r="W122" t="n">
         <v>0</v>
       </c>
-      <c r="X122" t="inlineStr"/>
+      <c r="X122" t="inlineStr">
+        <is>
+          <t>BA9233053</t>
+        </is>
+      </c>
       <c r="Y122" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -15978,7 +16462,7 @@
       <c r="Z122" t="inlineStr"/>
       <c r="AA122" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB122" t="n">
@@ -16097,7 +16581,11 @@
       <c r="W123" t="n">
         <v>0</v>
       </c>
-      <c r="X123" t="inlineStr"/>
+      <c r="X123" t="inlineStr">
+        <is>
+          <t>AA9611576</t>
+        </is>
+      </c>
       <c r="Y123" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16106,7 +16594,7 @@
       <c r="Z123" t="inlineStr"/>
       <c r="AA123" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB123" t="n">
@@ -16225,7 +16713,11 @@
       <c r="W124" t="n">
         <v>0</v>
       </c>
-      <c r="X124" t="inlineStr"/>
+      <c r="X124" t="inlineStr">
+        <is>
+          <t>AA9628484</t>
+        </is>
+      </c>
       <c r="Y124" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16234,7 +16726,7 @@
       <c r="Z124" t="inlineStr"/>
       <c r="AA124" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB124" t="n">
@@ -16353,7 +16845,11 @@
       <c r="W125" t="n">
         <v>0</v>
       </c>
-      <c r="X125" t="inlineStr"/>
+      <c r="X125" t="inlineStr">
+        <is>
+          <t>AA9621806</t>
+        </is>
+      </c>
       <c r="Y125" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16362,7 +16858,7 @@
       <c r="Z125" t="inlineStr"/>
       <c r="AA125" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB125" t="n">
@@ -16481,7 +16977,11 @@
       <c r="W126" t="n">
         <v>-19.5</v>
       </c>
-      <c r="X126" t="inlineStr"/>
+      <c r="X126" t="inlineStr">
+        <is>
+          <t>SA0125236</t>
+        </is>
+      </c>
       <c r="Y126" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16490,7 +16990,7 @@
       <c r="Z126" t="inlineStr"/>
       <c r="AA126" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB126" t="n">
@@ -16609,7 +17109,11 @@
       <c r="W127" t="n">
         <v>-19.5</v>
       </c>
-      <c r="X127" t="inlineStr"/>
+      <c r="X127" t="inlineStr">
+        <is>
+          <t>SA0125236</t>
+        </is>
+      </c>
       <c r="Y127" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16618,7 +17122,7 @@
       <c r="Z127" t="inlineStr"/>
       <c r="AA127" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB127" t="n">
@@ -16737,7 +17241,11 @@
       <c r="W128" t="n">
         <v>0</v>
       </c>
-      <c r="X128" t="inlineStr"/>
+      <c r="X128" t="inlineStr">
+        <is>
+          <t>ZH508457</t>
+        </is>
+      </c>
       <c r="Y128" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16746,7 +17254,7 @@
       <c r="Z128" t="inlineStr"/>
       <c r="AA128" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB128" t="n">
@@ -16865,7 +17373,11 @@
       <c r="W129" t="n">
         <v>0</v>
       </c>
-      <c r="X129" t="inlineStr"/>
+      <c r="X129" t="inlineStr">
+        <is>
+          <t>ZH508457</t>
+        </is>
+      </c>
       <c r="Y129" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -16874,7 +17386,7 @@
       <c r="Z129" t="inlineStr"/>
       <c r="AA129" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB129" t="n">
@@ -16993,7 +17505,11 @@
       <c r="W130" t="n">
         <v>0</v>
       </c>
-      <c r="X130" t="inlineStr"/>
+      <c r="X130" t="inlineStr">
+        <is>
+          <t>ZH509068</t>
+        </is>
+      </c>
       <c r="Y130" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17002,7 +17518,7 @@
       <c r="Z130" t="inlineStr"/>
       <c r="AA130" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB130" t="n">
@@ -17121,7 +17637,11 @@
       <c r="W131" t="n">
         <v>0</v>
       </c>
-      <c r="X131" t="inlineStr"/>
+      <c r="X131" t="inlineStr">
+        <is>
+          <t>J146806</t>
+        </is>
+      </c>
       <c r="Y131" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17130,7 +17650,7 @@
       <c r="Z131" t="inlineStr"/>
       <c r="AA131" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB131" t="n">
@@ -17249,7 +17769,11 @@
       <c r="W132" t="n">
         <v>0</v>
       </c>
-      <c r="X132" t="inlineStr"/>
+      <c r="X132" t="inlineStr">
+        <is>
+          <t>ZH501715</t>
+        </is>
+      </c>
       <c r="Y132" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17258,7 +17782,7 @@
       <c r="Z132" t="inlineStr"/>
       <c r="AA132" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB132" t="n">
@@ -17377,7 +17901,11 @@
       <c r="W133" t="n">
         <v>0</v>
       </c>
-      <c r="X133" t="inlineStr"/>
+      <c r="X133" t="inlineStr">
+        <is>
+          <t>ZH495903</t>
+        </is>
+      </c>
       <c r="Y133" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17386,7 +17914,7 @@
       <c r="Z133" t="inlineStr"/>
       <c r="AA133" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB133" t="n">
@@ -17505,7 +18033,11 @@
       <c r="W134" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="X134" t="inlineStr"/>
+      <c r="X134" t="inlineStr">
+        <is>
+          <t>ZH496376</t>
+        </is>
+      </c>
       <c r="Y134" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17514,7 +18046,7 @@
       <c r="Z134" t="inlineStr"/>
       <c r="AA134" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB134" t="n">
@@ -17633,7 +18165,11 @@
       <c r="W135" t="n">
         <v>0</v>
       </c>
-      <c r="X135" t="inlineStr"/>
+      <c r="X135" t="inlineStr">
+        <is>
+          <t>ZH504148</t>
+        </is>
+      </c>
       <c r="Y135" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17642,7 +18178,7 @@
       <c r="Z135" t="inlineStr"/>
       <c r="AA135" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB135" t="n">
@@ -17757,7 +18293,11 @@
       <c r="W136" t="n">
         <v>0</v>
       </c>
-      <c r="X136" t="inlineStr"/>
+      <c r="X136" t="inlineStr">
+        <is>
+          <t>ZH502582</t>
+        </is>
+      </c>
       <c r="Y136" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17766,7 +18306,7 @@
       <c r="Z136" t="inlineStr"/>
       <c r="AA136" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB136" t="n">
@@ -17885,7 +18425,11 @@
       <c r="W137" t="n">
         <v>0</v>
       </c>
-      <c r="X137" t="inlineStr"/>
+      <c r="X137" t="inlineStr">
+        <is>
+          <t>BA9222009</t>
+        </is>
+      </c>
       <c r="Y137" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -17894,7 +18438,7 @@
       <c r="Z137" t="inlineStr"/>
       <c r="AA137" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB137" t="n">
@@ -18013,7 +18557,11 @@
       <c r="W138" t="n">
         <v>0</v>
       </c>
-      <c r="X138" t="inlineStr"/>
+      <c r="X138" t="inlineStr">
+        <is>
+          <t>BA9217793</t>
+        </is>
+      </c>
       <c r="Y138" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18022,7 +18570,7 @@
       <c r="Z138" t="inlineStr"/>
       <c r="AA138" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB138" t="n">
@@ -18141,7 +18689,11 @@
       <c r="W139" t="n">
         <v>0</v>
       </c>
-      <c r="X139" t="inlineStr"/>
+      <c r="X139" t="inlineStr">
+        <is>
+          <t>AA9551307</t>
+        </is>
+      </c>
       <c r="Y139" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18150,7 +18702,7 @@
       <c r="Z139" t="inlineStr"/>
       <c r="AA139" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB139" t="n">
@@ -18265,7 +18817,11 @@
       <c r="W140" t="n">
         <v>0</v>
       </c>
-      <c r="X140" t="inlineStr"/>
+      <c r="X140" t="inlineStr">
+        <is>
+          <t>AA9550252</t>
+        </is>
+      </c>
       <c r="Y140" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18274,7 +18830,7 @@
       <c r="Z140" t="inlineStr"/>
       <c r="AA140" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB140" t="n">
@@ -18393,7 +18949,11 @@
       <c r="W141" t="n">
         <v>0</v>
       </c>
-      <c r="X141" t="inlineStr"/>
+      <c r="X141" t="inlineStr">
+        <is>
+          <t>AA9548715</t>
+        </is>
+      </c>
       <c r="Y141" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18402,7 +18962,7 @@
       <c r="Z141" t="inlineStr"/>
       <c r="AA141" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB141" t="n">
@@ -18521,7 +19081,11 @@
       <c r="W142" t="n">
         <v>0</v>
       </c>
-      <c r="X142" t="inlineStr"/>
+      <c r="X142" t="inlineStr">
+        <is>
+          <t>AA9548715</t>
+        </is>
+      </c>
       <c r="Y142" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18530,7 +19094,7 @@
       <c r="Z142" t="inlineStr"/>
       <c r="AA142" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB142" t="n">
@@ -18645,7 +19209,11 @@
       <c r="W143" t="n">
         <v>0</v>
       </c>
-      <c r="X143" t="inlineStr"/>
+      <c r="X143" t="inlineStr">
+        <is>
+          <t>AA9576113</t>
+        </is>
+      </c>
       <c r="Y143" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18654,7 +19222,7 @@
       <c r="Z143" t="inlineStr"/>
       <c r="AA143" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB143" t="n">
@@ -18773,7 +19341,11 @@
       <c r="W144" t="n">
         <v>0</v>
       </c>
-      <c r="X144" t="inlineStr"/>
+      <c r="X144" t="inlineStr">
+        <is>
+          <t>AA9566666</t>
+        </is>
+      </c>
       <c r="Y144" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18782,7 +19354,7 @@
       <c r="Z144" t="inlineStr"/>
       <c r="AA144" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB144" t="n">
@@ -18901,7 +19473,11 @@
       <c r="W145" t="n">
         <v>0</v>
       </c>
-      <c r="X145" t="inlineStr"/>
+      <c r="X145" t="inlineStr">
+        <is>
+          <t>BA9215882</t>
+        </is>
+      </c>
       <c r="Y145" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -18910,7 +19486,7 @@
       <c r="Z145" t="inlineStr"/>
       <c r="AA145" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB145" t="n">
@@ -19029,7 +19605,11 @@
       <c r="W146" t="n">
         <v>0</v>
       </c>
-      <c r="X146" t="inlineStr"/>
+      <c r="X146" t="inlineStr">
+        <is>
+          <t>BA9214984</t>
+        </is>
+      </c>
       <c r="Y146" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19038,7 +19618,7 @@
       <c r="Z146" t="inlineStr"/>
       <c r="AA146" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB146" t="n">
@@ -19157,7 +19737,11 @@
       <c r="W147" t="n">
         <v>0</v>
       </c>
-      <c r="X147" t="inlineStr"/>
+      <c r="X147" t="inlineStr">
+        <is>
+          <t>BA9214070</t>
+        </is>
+      </c>
       <c r="Y147" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19166,7 +19750,7 @@
       <c r="Z147" t="inlineStr"/>
       <c r="AA147" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB147" t="n">
@@ -19285,7 +19869,11 @@
       <c r="W148" t="n">
         <v>0</v>
       </c>
-      <c r="X148" t="inlineStr"/>
+      <c r="X148" t="inlineStr">
+        <is>
+          <t>BA9214009</t>
+        </is>
+      </c>
       <c r="Y148" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19294,7 +19882,7 @@
       <c r="Z148" t="inlineStr"/>
       <c r="AA148" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB148" t="n">
@@ -19413,7 +20001,11 @@
       <c r="W149" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X149" t="inlineStr"/>
+      <c r="X149" t="inlineStr">
+        <is>
+          <t>AA9550607</t>
+        </is>
+      </c>
       <c r="Y149" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19422,7 +20014,7 @@
       <c r="Z149" t="inlineStr"/>
       <c r="AA149" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB149" t="n">
@@ -19541,7 +20133,11 @@
       <c r="W150" t="n">
         <v>0</v>
       </c>
-      <c r="X150" t="inlineStr"/>
+      <c r="X150" t="inlineStr">
+        <is>
+          <t>BA9217262</t>
+        </is>
+      </c>
       <c r="Y150" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19550,7 +20146,7 @@
       <c r="Z150" t="inlineStr"/>
       <c r="AA150" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB150" t="n">
@@ -19669,7 +20265,11 @@
       <c r="W151" t="n">
         <v>0</v>
       </c>
-      <c r="X151" t="inlineStr"/>
+      <c r="X151" t="inlineStr">
+        <is>
+          <t>AA9547634</t>
+        </is>
+      </c>
       <c r="Y151" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19678,7 +20278,7 @@
       <c r="Z151" t="inlineStr"/>
       <c r="AA151" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB151" t="n">
@@ -19797,7 +20397,11 @@
       <c r="W152" t="n">
         <v>0</v>
       </c>
-      <c r="X152" t="inlineStr"/>
+      <c r="X152" t="inlineStr">
+        <is>
+          <t>AA9546432</t>
+        </is>
+      </c>
       <c r="Y152" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19806,7 +20410,7 @@
       <c r="Z152" t="inlineStr"/>
       <c r="AA152" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB152" t="n">
@@ -19921,7 +20525,11 @@
       <c r="W153" t="n">
         <v>0</v>
       </c>
-      <c r="X153" t="inlineStr"/>
+      <c r="X153" t="inlineStr">
+        <is>
+          <t>AA9555090</t>
+        </is>
+      </c>
       <c r="Y153" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -19930,7 +20538,7 @@
       <c r="Z153" t="inlineStr"/>
       <c r="AA153" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB153" t="n">
@@ -20049,7 +20657,11 @@
       <c r="W154" t="n">
         <v>0</v>
       </c>
-      <c r="X154" t="inlineStr"/>
+      <c r="X154" t="inlineStr">
+        <is>
+          <t>AA9565464</t>
+        </is>
+      </c>
       <c r="Y154" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20058,7 +20670,7 @@
       <c r="Z154" t="inlineStr"/>
       <c r="AA154" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB154" t="n">
@@ -20177,7 +20789,11 @@
       <c r="W155" t="n">
         <v>0</v>
       </c>
-      <c r="X155" t="inlineStr"/>
+      <c r="X155" t="inlineStr">
+        <is>
+          <t>AA9540830</t>
+        </is>
+      </c>
       <c r="Y155" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20186,7 +20802,7 @@
       <c r="Z155" t="inlineStr"/>
       <c r="AA155" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB155" t="n">
@@ -20305,7 +20921,11 @@
       <c r="W156" t="n">
         <v>0</v>
       </c>
-      <c r="X156" t="inlineStr"/>
+      <c r="X156" t="inlineStr">
+        <is>
+          <t>AA9563154</t>
+        </is>
+      </c>
       <c r="Y156" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20314,7 +20934,7 @@
       <c r="Z156" t="inlineStr"/>
       <c r="AA156" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB156" t="n">
@@ -20433,7 +21053,11 @@
       <c r="W157" t="n">
         <v>0</v>
       </c>
-      <c r="X157" t="inlineStr"/>
+      <c r="X157" t="inlineStr">
+        <is>
+          <t>AA9546575</t>
+        </is>
+      </c>
       <c r="Y157" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20442,7 +21066,7 @@
       <c r="Z157" t="inlineStr"/>
       <c r="AA157" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB157" t="n">
@@ -20561,7 +21185,11 @@
       <c r="W158" t="n">
         <v>0</v>
       </c>
-      <c r="X158" t="inlineStr"/>
+      <c r="X158" t="inlineStr">
+        <is>
+          <t>223150301109202</t>
+        </is>
+      </c>
       <c r="Y158" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20570,7 +21198,7 @@
       <c r="Z158" t="inlineStr"/>
       <c r="AA158" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB158" t="n">
@@ -20689,7 +21317,11 @@
       <c r="W159" t="n">
         <v>0</v>
       </c>
-      <c r="X159" t="inlineStr"/>
+      <c r="X159" t="inlineStr">
+        <is>
+          <t>223150301109202</t>
+        </is>
+      </c>
       <c r="Y159" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20698,7 +21330,7 @@
       <c r="Z159" t="inlineStr"/>
       <c r="AA159" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB159" t="n">
@@ -20817,7 +21449,11 @@
       <c r="W160" t="n">
         <v>0</v>
       </c>
-      <c r="X160" t="inlineStr"/>
+      <c r="X160" t="inlineStr">
+        <is>
+          <t>ZH489292</t>
+        </is>
+      </c>
       <c r="Y160" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20826,7 +21462,7 @@
       <c r="Z160" t="inlineStr"/>
       <c r="AA160" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB160" t="n">
@@ -20945,7 +21581,11 @@
       <c r="W161" t="n">
         <v>0</v>
       </c>
-      <c r="X161" t="inlineStr"/>
+      <c r="X161" t="inlineStr">
+        <is>
+          <t>ZH489691</t>
+        </is>
+      </c>
       <c r="Y161" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -20954,7 +21594,7 @@
       <c r="Z161" t="inlineStr"/>
       <c r="AA161" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB161" t="n">
@@ -21069,7 +21709,11 @@
       <c r="W162" t="n">
         <v>0</v>
       </c>
-      <c r="X162" t="inlineStr"/>
+      <c r="X162" t="inlineStr">
+        <is>
+          <t>113150306459548</t>
+        </is>
+      </c>
       <c r="Y162" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21078,7 +21722,7 @@
       <c r="Z162" t="inlineStr"/>
       <c r="AA162" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB162" t="n">
@@ -21197,7 +21841,11 @@
       <c r="W163" t="n">
         <v>0</v>
       </c>
-      <c r="X163" t="inlineStr"/>
+      <c r="X163" t="inlineStr">
+        <is>
+          <t>113150306459332</t>
+        </is>
+      </c>
       <c r="Y163" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21206,7 +21854,7 @@
       <c r="Z163" t="inlineStr"/>
       <c r="AA163" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB163" t="n">
@@ -21321,7 +21969,11 @@
       <c r="W164" t="n">
         <v>0</v>
       </c>
-      <c r="X164" t="inlineStr"/>
+      <c r="X164" t="inlineStr">
+        <is>
+          <t>113150306459319</t>
+        </is>
+      </c>
       <c r="Y164" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21330,7 +21982,7 @@
       <c r="Z164" t="inlineStr"/>
       <c r="AA164" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB164" t="n">
@@ -21445,7 +22097,11 @@
       <c r="W165" t="n">
         <v>0</v>
       </c>
-      <c r="X165" t="inlineStr"/>
+      <c r="X165" t="inlineStr">
+        <is>
+          <t>113150306459319</t>
+        </is>
+      </c>
       <c r="Y165" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21454,7 +22110,7 @@
       <c r="Z165" t="inlineStr"/>
       <c r="AA165" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB165" t="n">
@@ -21573,7 +22229,11 @@
       <c r="W166" t="n">
         <v>0</v>
       </c>
-      <c r="X166" t="inlineStr"/>
+      <c r="X166" t="inlineStr">
+        <is>
+          <t>BA9208442</t>
+        </is>
+      </c>
       <c r="Y166" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21582,7 +22242,7 @@
       <c r="Z166" t="inlineStr"/>
       <c r="AA166" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB166" t="n">
@@ -21701,7 +22361,11 @@
       <c r="W167" t="n">
         <v>0</v>
       </c>
-      <c r="X167" t="inlineStr"/>
+      <c r="X167" t="inlineStr">
+        <is>
+          <t>BA9209397</t>
+        </is>
+      </c>
       <c r="Y167" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21710,7 +22374,7 @@
       <c r="Z167" t="inlineStr"/>
       <c r="AA167" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB167" t="n">
@@ -21829,7 +22493,11 @@
       <c r="W168" t="n">
         <v>0</v>
       </c>
-      <c r="X168" t="inlineStr"/>
+      <c r="X168" t="inlineStr">
+        <is>
+          <t>AA9520478</t>
+        </is>
+      </c>
       <c r="Y168" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21838,7 +22506,7 @@
       <c r="Z168" t="inlineStr"/>
       <c r="AA168" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB168" t="n">
@@ -21957,7 +22625,11 @@
       <c r="W169" t="n">
         <v>0</v>
       </c>
-      <c r="X169" t="inlineStr"/>
+      <c r="X169" t="inlineStr">
+        <is>
+          <t>AA9535581</t>
+        </is>
+      </c>
       <c r="Y169" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -21966,7 +22638,7 @@
       <c r="Z169" t="inlineStr"/>
       <c r="AA169" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB169" t="n">
@@ -22085,7 +22757,11 @@
       <c r="W170" t="n">
         <v>0</v>
       </c>
-      <c r="X170" t="inlineStr"/>
+      <c r="X170" t="inlineStr">
+        <is>
+          <t>AA9522280</t>
+        </is>
+      </c>
       <c r="Y170" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22094,7 +22770,7 @@
       <c r="Z170" t="inlineStr"/>
       <c r="AA170" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB170" t="n">
@@ -22213,7 +22889,11 @@
       <c r="W171" t="n">
         <v>0</v>
       </c>
-      <c r="X171" t="inlineStr"/>
+      <c r="X171" t="inlineStr">
+        <is>
+          <t>BA9205379</t>
+        </is>
+      </c>
       <c r="Y171" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22222,7 +22902,7 @@
       <c r="Z171" t="inlineStr"/>
       <c r="AA171" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB171" t="n">
@@ -22337,7 +23017,11 @@
       <c r="W172" t="n">
         <v>0</v>
       </c>
-      <c r="X172" t="inlineStr"/>
+      <c r="X172" t="inlineStr">
+        <is>
+          <t>BA9206989</t>
+        </is>
+      </c>
       <c r="Y172" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22346,7 +23030,7 @@
       <c r="Z172" t="inlineStr"/>
       <c r="AA172" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB172" t="n">
@@ -22465,7 +23149,11 @@
       <c r="W173" t="n">
         <v>0</v>
       </c>
-      <c r="X173" t="inlineStr"/>
+      <c r="X173" t="inlineStr">
+        <is>
+          <t>AA9494776</t>
+        </is>
+      </c>
       <c r="Y173" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22474,7 +23162,7 @@
       <c r="Z173" t="inlineStr"/>
       <c r="AA173" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB173" t="n">
@@ -22593,7 +23281,11 @@
       <c r="W174" t="n">
         <v>0</v>
       </c>
-      <c r="X174" t="inlineStr"/>
+      <c r="X174" t="inlineStr">
+        <is>
+          <t>AA9500557</t>
+        </is>
+      </c>
       <c r="Y174" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22602,7 +23294,7 @@
       <c r="Z174" t="inlineStr"/>
       <c r="AA174" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB174" t="n">
@@ -22721,7 +23413,11 @@
       <c r="W175" t="n">
         <v>0</v>
       </c>
-      <c r="X175" t="inlineStr"/>
+      <c r="X175" t="inlineStr">
+        <is>
+          <t>BA9203301</t>
+        </is>
+      </c>
       <c r="Y175" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22730,7 +23426,7 @@
       <c r="Z175" t="inlineStr"/>
       <c r="AA175" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB175" t="n">
@@ -22849,7 +23545,11 @@
       <c r="W176" t="n">
         <v>0</v>
       </c>
-      <c r="X176" t="inlineStr"/>
+      <c r="X176" t="inlineStr">
+        <is>
+          <t>AA9485210</t>
+        </is>
+      </c>
       <c r="Y176" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22858,7 +23558,7 @@
       <c r="Z176" t="inlineStr"/>
       <c r="AA176" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB176" t="n">
@@ -22977,7 +23677,11 @@
       <c r="W177" t="n">
         <v>0</v>
       </c>
-      <c r="X177" t="inlineStr"/>
+      <c r="X177" t="inlineStr">
+        <is>
+          <t>AA9497436</t>
+        </is>
+      </c>
       <c r="Y177" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -22986,7 +23690,7 @@
       <c r="Z177" t="inlineStr"/>
       <c r="AA177" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB177" t="n">
@@ -23105,7 +23809,11 @@
       <c r="W178" t="n">
         <v>0</v>
       </c>
-      <c r="X178" t="inlineStr"/>
+      <c r="X178" t="inlineStr">
+        <is>
+          <t>AA9489171</t>
+        </is>
+      </c>
       <c r="Y178" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23114,7 +23822,7 @@
       <c r="Z178" t="inlineStr"/>
       <c r="AA178" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB178" t="n">
@@ -23229,7 +23937,11 @@
       <c r="W179" t="n">
         <v>0</v>
       </c>
-      <c r="X179" t="inlineStr"/>
+      <c r="X179" t="inlineStr">
+        <is>
+          <t>J135995</t>
+        </is>
+      </c>
       <c r="Y179" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23238,7 +23950,7 @@
       <c r="Z179" t="inlineStr"/>
       <c r="AA179" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB179" t="n">
@@ -23357,7 +24069,11 @@
       <c r="W180" t="n">
         <v>0</v>
       </c>
-      <c r="X180" t="inlineStr"/>
+      <c r="X180" t="inlineStr">
+        <is>
+          <t>AA9480848</t>
+        </is>
+      </c>
       <c r="Y180" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23366,7 +24082,7 @@
       <c r="Z180" t="inlineStr"/>
       <c r="AA180" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB180" t="n">
@@ -23485,7 +24201,11 @@
       <c r="W181" t="n">
         <v>0</v>
       </c>
-      <c r="X181" t="inlineStr"/>
+      <c r="X181" t="inlineStr">
+        <is>
+          <t>113150306457207</t>
+        </is>
+      </c>
       <c r="Y181" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23494,7 +24214,7 @@
       <c r="Z181" t="inlineStr"/>
       <c r="AA181" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB181" t="n">
@@ -23613,7 +24333,11 @@
       <c r="W182" t="n">
         <v>0</v>
       </c>
-      <c r="X182" t="inlineStr"/>
+      <c r="X182" t="inlineStr">
+        <is>
+          <t>113150306457189</t>
+        </is>
+      </c>
       <c r="Y182" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23622,7 +24346,7 @@
       <c r="Z182" t="inlineStr"/>
       <c r="AA182" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB182" t="n">
@@ -23741,7 +24465,11 @@
       <c r="W183" t="n">
         <v>-6.22</v>
       </c>
-      <c r="X183" t="inlineStr"/>
+      <c r="X183" t="inlineStr">
+        <is>
+          <t>ZH475696</t>
+        </is>
+      </c>
       <c r="Y183" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23750,7 +24478,7 @@
       <c r="Z183" t="inlineStr"/>
       <c r="AA183" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB183" t="n">
@@ -23869,7 +24597,11 @@
       <c r="W184" t="n">
         <v>-6.23</v>
       </c>
-      <c r="X184" t="inlineStr"/>
+      <c r="X184" t="inlineStr">
+        <is>
+          <t>ZH475696</t>
+        </is>
+      </c>
       <c r="Y184" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -23878,7 +24610,7 @@
       <c r="Z184" t="inlineStr"/>
       <c r="AA184" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB184" t="n">
@@ -23997,7 +24729,11 @@
       <c r="W185" t="n">
         <v>0</v>
       </c>
-      <c r="X185" t="inlineStr"/>
+      <c r="X185" t="inlineStr">
+        <is>
+          <t>ZH478267</t>
+        </is>
+      </c>
       <c r="Y185" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24006,7 +24742,7 @@
       <c r="Z185" t="inlineStr"/>
       <c r="AA185" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB185" t="n">
@@ -24125,7 +24861,11 @@
       <c r="W186" t="n">
         <v>0</v>
       </c>
-      <c r="X186" t="inlineStr"/>
+      <c r="X186" t="inlineStr">
+        <is>
+          <t>ZH474974</t>
+        </is>
+      </c>
       <c r="Y186" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24134,7 +24874,7 @@
       <c r="Z186" t="inlineStr"/>
       <c r="AA186" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB186" t="n">
@@ -24253,7 +24993,11 @@
       <c r="W187" t="n">
         <v>0</v>
       </c>
-      <c r="X187" t="inlineStr"/>
+      <c r="X187" t="inlineStr">
+        <is>
+          <t>ZH479745</t>
+        </is>
+      </c>
       <c r="Y187" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24262,7 +25006,7 @@
       <c r="Z187" t="inlineStr"/>
       <c r="AA187" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB187" t="n">
@@ -24377,7 +25121,11 @@
       <c r="W188" t="n">
         <v>0</v>
       </c>
-      <c r="X188" t="inlineStr"/>
+      <c r="X188" t="inlineStr">
+        <is>
+          <t>AA9470313</t>
+        </is>
+      </c>
       <c r="Y188" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24386,7 +25134,7 @@
       <c r="Z188" t="inlineStr"/>
       <c r="AA188" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB188" t="n">
@@ -24505,7 +25253,11 @@
       <c r="W189" t="n">
         <v>0</v>
       </c>
-      <c r="X189" t="inlineStr"/>
+      <c r="X189" t="inlineStr">
+        <is>
+          <t>BA9196718</t>
+        </is>
+      </c>
       <c r="Y189" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24514,7 +25266,7 @@
       <c r="Z189" t="inlineStr"/>
       <c r="AA189" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB189" t="n">
@@ -24633,7 +25385,11 @@
       <c r="W190" t="n">
         <v>0</v>
       </c>
-      <c r="X190" t="inlineStr"/>
+      <c r="X190" t="inlineStr">
+        <is>
+          <t>BA9192143</t>
+        </is>
+      </c>
       <c r="Y190" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24642,7 +25398,7 @@
       <c r="Z190" t="inlineStr"/>
       <c r="AA190" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB190" t="n">
@@ -24761,7 +25517,11 @@
       <c r="W191" t="n">
         <v>0</v>
       </c>
-      <c r="X191" t="inlineStr"/>
+      <c r="X191" t="inlineStr">
+        <is>
+          <t>BA9190770</t>
+        </is>
+      </c>
       <c r="Y191" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24770,7 +25530,7 @@
       <c r="Z191" t="inlineStr"/>
       <c r="AA191" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB191" t="n">
@@ -24889,7 +25649,11 @@
       <c r="W192" t="n">
         <v>0</v>
       </c>
-      <c r="X192" t="inlineStr"/>
+      <c r="X192" t="inlineStr">
+        <is>
+          <t>BA9196116</t>
+        </is>
+      </c>
       <c r="Y192" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -24898,7 +25662,7 @@
       <c r="Z192" t="inlineStr"/>
       <c r="AA192" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB192" t="n">
@@ -25017,7 +25781,11 @@
       <c r="W193" t="n">
         <v>0</v>
       </c>
-      <c r="X193" t="inlineStr"/>
+      <c r="X193" t="inlineStr">
+        <is>
+          <t>BA9196116</t>
+        </is>
+      </c>
       <c r="Y193" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25026,7 +25794,7 @@
       <c r="Z193" t="inlineStr"/>
       <c r="AA193" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB193" t="n">
@@ -25145,7 +25913,11 @@
       <c r="W194" t="n">
         <v>0</v>
       </c>
-      <c r="X194" t="inlineStr"/>
+      <c r="X194" t="inlineStr">
+        <is>
+          <t>BA9191790</t>
+        </is>
+      </c>
       <c r="Y194" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25154,7 +25926,7 @@
       <c r="Z194" t="inlineStr"/>
       <c r="AA194" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB194" t="n">
@@ -25273,7 +26045,11 @@
       <c r="W195" t="n">
         <v>0</v>
       </c>
-      <c r="X195" t="inlineStr"/>
+      <c r="X195" t="inlineStr">
+        <is>
+          <t>BA9191790</t>
+        </is>
+      </c>
       <c r="Y195" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25282,7 +26058,7 @@
       <c r="Z195" t="inlineStr"/>
       <c r="AA195" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB195" t="n">
@@ -25401,7 +26177,11 @@
       <c r="W196" t="n">
         <v>0</v>
       </c>
-      <c r="X196" t="inlineStr"/>
+      <c r="X196" t="inlineStr">
+        <is>
+          <t>BA9195655</t>
+        </is>
+      </c>
       <c r="Y196" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25410,7 +26190,7 @@
       <c r="Z196" t="inlineStr"/>
       <c r="AA196" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB196" t="n">
@@ -25525,7 +26305,11 @@
       <c r="W197" t="n">
         <v>0</v>
       </c>
-      <c r="X197" t="inlineStr"/>
+      <c r="X197" t="inlineStr">
+        <is>
+          <t>BA9190199</t>
+        </is>
+      </c>
       <c r="Y197" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25534,7 +26318,7 @@
       <c r="Z197" t="inlineStr"/>
       <c r="AA197" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB197" t="n">
@@ -25653,7 +26437,11 @@
       <c r="W198" t="n">
         <v>0</v>
       </c>
-      <c r="X198" t="inlineStr"/>
+      <c r="X198" t="inlineStr">
+        <is>
+          <t>BA9195110</t>
+        </is>
+      </c>
       <c r="Y198" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25662,7 +26450,7 @@
       <c r="Z198" t="inlineStr"/>
       <c r="AA198" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB198" t="n">
@@ -25781,7 +26569,11 @@
       <c r="W199" t="n">
         <v>0</v>
       </c>
-      <c r="X199" t="inlineStr"/>
+      <c r="X199" t="inlineStr">
+        <is>
+          <t>223150301107083</t>
+        </is>
+      </c>
       <c r="Y199" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25790,7 +26582,7 @@
       <c r="Z199" t="inlineStr"/>
       <c r="AA199" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB199" t="n">
@@ -25909,7 +26701,11 @@
       <c r="W200" t="n">
         <v>0</v>
       </c>
-      <c r="X200" t="inlineStr"/>
+      <c r="X200" t="inlineStr">
+        <is>
+          <t>223150301107523</t>
+        </is>
+      </c>
       <c r="Y200" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -25918,7 +26714,7 @@
       <c r="Z200" t="inlineStr"/>
       <c r="AA200" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB200" t="n">
@@ -26037,7 +26833,11 @@
       <c r="W201" t="n">
         <v>0</v>
       </c>
-      <c r="X201" t="inlineStr"/>
+      <c r="X201" t="inlineStr">
+        <is>
+          <t>223150301107523</t>
+        </is>
+      </c>
       <c r="Y201" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26046,7 +26846,7 @@
       <c r="Z201" t="inlineStr"/>
       <c r="AA201" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB201" t="n">
@@ -26161,7 +26961,11 @@
       <c r="W202" t="n">
         <v>0</v>
       </c>
-      <c r="X202" t="inlineStr"/>
+      <c r="X202" t="inlineStr">
+        <is>
+          <t>AA9427572</t>
+        </is>
+      </c>
       <c r="Y202" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26170,7 +26974,7 @@
       <c r="Z202" t="inlineStr"/>
       <c r="AA202" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB202" t="n">
@@ -26285,7 +27089,11 @@
       <c r="W203" t="n">
         <v>0</v>
       </c>
-      <c r="X203" t="inlineStr"/>
+      <c r="X203" t="inlineStr">
+        <is>
+          <t>113150306447828</t>
+        </is>
+      </c>
       <c r="Y203" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26294,7 +27102,7 @@
       <c r="Z203" t="inlineStr"/>
       <c r="AA203" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB203" t="n">
@@ -26413,7 +27221,11 @@
       <c r="W204" t="n">
         <v>0</v>
       </c>
-      <c r="X204" t="inlineStr"/>
+      <c r="X204" t="inlineStr">
+        <is>
+          <t>AA9424151</t>
+        </is>
+      </c>
       <c r="Y204" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26422,7 +27234,7 @@
       <c r="Z204" t="inlineStr"/>
       <c r="AA204" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB204" t="n">
@@ -26541,7 +27353,11 @@
       <c r="W205" t="n">
         <v>0</v>
       </c>
-      <c r="X205" t="inlineStr"/>
+      <c r="X205" t="inlineStr">
+        <is>
+          <t>AA9427258</t>
+        </is>
+      </c>
       <c r="Y205" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26550,7 +27366,7 @@
       <c r="Z205" t="inlineStr"/>
       <c r="AA205" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB205" t="n">
@@ -26669,7 +27485,11 @@
       <c r="W206" t="n">
         <v>0</v>
       </c>
-      <c r="X206" t="inlineStr"/>
+      <c r="X206" t="inlineStr">
+        <is>
+          <t>AA9427403</t>
+        </is>
+      </c>
       <c r="Y206" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26678,7 +27498,7 @@
       <c r="Z206" t="inlineStr"/>
       <c r="AA206" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB206" t="n">
@@ -26797,7 +27617,11 @@
       <c r="W207" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="X207" t="inlineStr"/>
+      <c r="X207" t="inlineStr">
+        <is>
+          <t>J130540</t>
+        </is>
+      </c>
       <c r="Y207" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26806,7 +27630,7 @@
       <c r="Z207" t="inlineStr"/>
       <c r="AA207" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB207" t="n">
@@ -26925,7 +27749,11 @@
       <c r="W208" t="n">
         <v>-24.9</v>
       </c>
-      <c r="X208" t="inlineStr"/>
+      <c r="X208" t="inlineStr">
+        <is>
+          <t>J129505</t>
+        </is>
+      </c>
       <c r="Y208" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -26934,7 +27762,7 @@
       <c r="Z208" t="inlineStr"/>
       <c r="AA208" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB208" t="n">
@@ -27053,7 +27881,11 @@
       <c r="W209" t="n">
         <v>0</v>
       </c>
-      <c r="X209" t="inlineStr"/>
+      <c r="X209" t="inlineStr">
+        <is>
+          <t>J130213</t>
+        </is>
+      </c>
       <c r="Y209" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27062,7 +27894,7 @@
       <c r="Z209" t="inlineStr"/>
       <c r="AA209" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB209" t="n">
@@ -27181,7 +28013,11 @@
       <c r="W210" t="n">
         <v>0</v>
       </c>
-      <c r="X210" t="inlineStr"/>
+      <c r="X210" t="inlineStr">
+        <is>
+          <t>ZH463252</t>
+        </is>
+      </c>
       <c r="Y210" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27190,7 +28026,7 @@
       <c r="Z210" t="inlineStr"/>
       <c r="AA210" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB210" t="n">
@@ -27309,7 +28145,11 @@
       <c r="W211" t="n">
         <v>0</v>
       </c>
-      <c r="X211" t="inlineStr"/>
+      <c r="X211" t="inlineStr">
+        <is>
+          <t>ZH463252</t>
+        </is>
+      </c>
       <c r="Y211" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27318,7 +28158,7 @@
       <c r="Z211" t="inlineStr"/>
       <c r="AA211" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB211" t="n">
@@ -27437,7 +28277,11 @@
       <c r="W212" t="n">
         <v>0</v>
       </c>
-      <c r="X212" t="inlineStr"/>
+      <c r="X212" t="inlineStr">
+        <is>
+          <t>ZH459920</t>
+        </is>
+      </c>
       <c r="Y212" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27446,7 +28290,7 @@
       <c r="Z212" t="inlineStr"/>
       <c r="AA212" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB212" t="n">
@@ -27565,7 +28409,11 @@
       <c r="W213" t="n">
         <v>0</v>
       </c>
-      <c r="X213" t="inlineStr"/>
+      <c r="X213" t="inlineStr">
+        <is>
+          <t>BA9177407</t>
+        </is>
+      </c>
       <c r="Y213" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27574,7 +28422,7 @@
       <c r="Z213" t="inlineStr"/>
       <c r="AA213" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB213" t="n">
@@ -27693,7 +28541,11 @@
       <c r="W214" t="n">
         <v>0</v>
       </c>
-      <c r="X214" t="inlineStr"/>
+      <c r="X214" t="inlineStr">
+        <is>
+          <t>BA9177407</t>
+        </is>
+      </c>
       <c r="Y214" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27702,7 +28554,7 @@
       <c r="Z214" t="inlineStr"/>
       <c r="AA214" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB214" t="n">
@@ -27821,7 +28673,11 @@
       <c r="W215" t="n">
         <v>0</v>
       </c>
-      <c r="X215" t="inlineStr"/>
+      <c r="X215" t="inlineStr">
+        <is>
+          <t>BA9180296</t>
+        </is>
+      </c>
       <c r="Y215" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27830,7 +28686,7 @@
       <c r="Z215" t="inlineStr"/>
       <c r="AA215" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB215" t="n">
@@ -27949,7 +28805,11 @@
       <c r="W216" t="n">
         <v>0</v>
       </c>
-      <c r="X216" t="inlineStr"/>
+      <c r="X216" t="inlineStr">
+        <is>
+          <t>BA9184257</t>
+        </is>
+      </c>
       <c r="Y216" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -27958,7 +28818,7 @@
       <c r="Z216" t="inlineStr"/>
       <c r="AA216" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB216" t="n">
@@ -28077,7 +28937,11 @@
       <c r="W217" t="n">
         <v>0</v>
       </c>
-      <c r="X217" t="inlineStr"/>
+      <c r="X217" t="inlineStr">
+        <is>
+          <t>K602576</t>
+        </is>
+      </c>
       <c r="Y217" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28086,7 +28950,7 @@
       <c r="Z217" t="inlineStr"/>
       <c r="AA217" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB217" t="n">
@@ -28205,7 +29069,11 @@
       <c r="W218" t="n">
         <v>0</v>
       </c>
-      <c r="X218" t="inlineStr"/>
+      <c r="X218" t="inlineStr">
+        <is>
+          <t>BA9185424</t>
+        </is>
+      </c>
       <c r="Y218" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28214,7 +29082,7 @@
       <c r="Z218" t="inlineStr"/>
       <c r="AA218" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB218" t="n">
@@ -28333,7 +29201,11 @@
       <c r="W219" t="n">
         <v>0</v>
       </c>
-      <c r="X219" t="inlineStr"/>
+      <c r="X219" t="inlineStr">
+        <is>
+          <t>BA9185256</t>
+        </is>
+      </c>
       <c r="Y219" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28342,7 +29214,7 @@
       <c r="Z219" t="inlineStr"/>
       <c r="AA219" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB219" t="n">
@@ -28461,7 +29333,11 @@
       <c r="W220" t="n">
         <v>0</v>
       </c>
-      <c r="X220" t="inlineStr"/>
+      <c r="X220" t="inlineStr">
+        <is>
+          <t>BA9179051</t>
+        </is>
+      </c>
       <c r="Y220" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28470,7 +29346,7 @@
       <c r="Z220" t="inlineStr"/>
       <c r="AA220" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB220" t="n">
@@ -28589,7 +29465,11 @@
       <c r="W221" t="n">
         <v>0</v>
       </c>
-      <c r="X221" t="inlineStr"/>
+      <c r="X221" t="inlineStr">
+        <is>
+          <t>BA9179051</t>
+        </is>
+      </c>
       <c r="Y221" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28598,7 +29478,7 @@
       <c r="Z221" t="inlineStr"/>
       <c r="AA221" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB221" t="n">
@@ -28717,7 +29597,11 @@
       <c r="W222" t="n">
         <v>0</v>
       </c>
-      <c r="X222" t="inlineStr"/>
+      <c r="X222" t="inlineStr">
+        <is>
+          <t>BA9179051</t>
+        </is>
+      </c>
       <c r="Y222" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28726,7 +29610,7 @@
       <c r="Z222" t="inlineStr"/>
       <c r="AA222" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB222" t="n">
@@ -28845,7 +29729,11 @@
       <c r="W223" t="n">
         <v>0</v>
       </c>
-      <c r="X223" t="inlineStr"/>
+      <c r="X223" t="inlineStr">
+        <is>
+          <t>BA9179051</t>
+        </is>
+      </c>
       <c r="Y223" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28854,7 +29742,7 @@
       <c r="Z223" t="inlineStr"/>
       <c r="AA223" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB223" t="n">
@@ -28973,7 +29861,11 @@
       <c r="W224" t="n">
         <v>0</v>
       </c>
-      <c r="X224" t="inlineStr"/>
+      <c r="X224" t="inlineStr">
+        <is>
+          <t>BA9185241</t>
+        </is>
+      </c>
       <c r="Y224" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -28982,7 +29874,7 @@
       <c r="Z224" t="inlineStr"/>
       <c r="AA224" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB224" t="n">
@@ -29101,7 +29993,11 @@
       <c r="W225" t="n">
         <v>0</v>
       </c>
-      <c r="X225" t="inlineStr"/>
+      <c r="X225" t="inlineStr">
+        <is>
+          <t>BA9186937</t>
+        </is>
+      </c>
       <c r="Y225" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -29110,7 +30006,7 @@
       <c r="Z225" t="inlineStr"/>
       <c r="AA225" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB225" t="n">
@@ -29229,7 +30125,11 @@
       <c r="W226" t="n">
         <v>0</v>
       </c>
-      <c r="X226" t="inlineStr"/>
+      <c r="X226" t="inlineStr">
+        <is>
+          <t>BA9179167</t>
+        </is>
+      </c>
       <c r="Y226" t="inlineStr">
         <is>
           <t>Amazon.com.tr</t>
@@ -29238,7 +30138,7 @@
       <c r="Z226" t="inlineStr"/>
       <c r="AA226" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>08/01/2024</t>
         </is>
       </c>
       <c r="AB226" t="n">

</xml_diff>

<commit_message>
Updated the empty values in INVOICE_COUNTY column
</commit_message>
<xml_diff>
--- a/processed_file.xlsx
+++ b/processed_file.xlsx
@@ -669,7 +669,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -698,7 +698,7 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB2" t="n">
@@ -801,7 +801,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -830,7 +830,7 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB3" t="n">
@@ -933,7 +933,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -962,7 +962,7 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB4" t="n">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1094,7 +1094,7 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB5" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1226,7 +1226,7 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB6" t="n">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1358,7 +1358,7 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB7" t="n">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1490,7 +1490,7 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB8" t="n">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1622,7 +1622,7 @@
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB9" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1754,7 +1754,7 @@
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB10" t="n">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -1886,7 +1886,7 @@
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB11" t="n">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2018,7 +2018,7 @@
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB12" t="n">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -2146,7 +2146,7 @@
       <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB13" t="n">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -2278,7 +2278,7 @@
       <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB14" t="n">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
@@ -2410,7 +2410,7 @@
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB15" t="n">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
@@ -2542,7 +2542,7 @@
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB16" t="n">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
@@ -2670,7 +2670,7 @@
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB17" t="n">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2802,7 +2802,7 @@
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB18" t="n">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
@@ -2934,7 +2934,7 @@
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB19" t="n">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -3066,7 +3066,7 @@
       <c r="Z20" t="inlineStr"/>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB20" t="n">
@@ -3169,7 +3169,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
@@ -3198,7 +3198,7 @@
       <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB21" t="n">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -3330,7 +3330,7 @@
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB22" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3462,7 +3462,7 @@
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB23" t="n">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -3594,7 +3594,7 @@
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB24" t="n">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -3726,7 +3726,7 @@
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB25" t="n">
@@ -3829,7 +3829,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -3858,7 +3858,7 @@
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB26" t="n">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
@@ -3990,7 +3990,7 @@
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB27" t="n">
@@ -4093,7 +4093,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -4122,7 +4122,7 @@
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB28" t="n">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
@@ -4254,7 +4254,7 @@
       <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB29" t="n">
@@ -4357,7 +4357,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
@@ -4386,7 +4386,7 @@
       <c r="Z30" t="inlineStr"/>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB30" t="n">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
@@ -4518,7 +4518,7 @@
       <c r="Z31" t="inlineStr"/>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB31" t="n">
@@ -4650,7 +4650,7 @@
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB32" t="n">
@@ -4782,7 +4782,7 @@
       <c r="Z33" t="inlineStr"/>
       <c r="AA33" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB33" t="n">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
@@ -4914,7 +4914,7 @@
       <c r="Z34" t="inlineStr"/>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB34" t="n">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
@@ -5046,7 +5046,7 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB35" t="n">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
@@ -5178,7 +5178,7 @@
       <c r="Z36" t="inlineStr"/>
       <c r="AA36" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB36" t="n">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U37" t="inlineStr">
@@ -5310,7 +5310,7 @@
       <c r="Z37" t="inlineStr"/>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB37" t="n">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
@@ -5442,7 +5442,7 @@
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB38" t="n">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
@@ -5574,7 +5574,7 @@
       <c r="Z39" t="inlineStr"/>
       <c r="AA39" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB39" t="n">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U40" t="inlineStr">
@@ -5706,7 +5706,7 @@
       <c r="Z40" t="inlineStr"/>
       <c r="AA40" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB40" t="n">
@@ -5809,7 +5809,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U41" t="inlineStr">
@@ -5838,7 +5838,7 @@
       <c r="Z41" t="inlineStr"/>
       <c r="AA41" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB41" t="n">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U42" t="inlineStr">
@@ -5970,7 +5970,7 @@
       <c r="Z42" t="inlineStr"/>
       <c r="AA42" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB42" t="n">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U43" t="inlineStr">
@@ -6102,7 +6102,7 @@
       <c r="Z43" t="inlineStr"/>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB43" t="n">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U44" t="inlineStr">
@@ -6234,7 +6234,7 @@
       <c r="Z44" t="inlineStr"/>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB44" t="n">
@@ -6333,7 +6333,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U45" t="inlineStr">
@@ -6362,7 +6362,7 @@
       <c r="Z45" t="inlineStr"/>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB45" t="n">
@@ -6465,7 +6465,7 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U46" t="inlineStr">
@@ -6494,7 +6494,7 @@
       <c r="Z46" t="inlineStr"/>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB46" t="n">
@@ -6597,7 +6597,7 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U47" t="inlineStr">
@@ -6626,7 +6626,7 @@
       <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB47" t="n">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U48" t="inlineStr">
@@ -6758,7 +6758,7 @@
       <c r="Z48" t="inlineStr"/>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB48" t="n">
@@ -6857,7 +6857,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U49" t="inlineStr">
@@ -6886,7 +6886,7 @@
       <c r="Z49" t="inlineStr"/>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB49" t="n">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U50" t="inlineStr">
@@ -7014,7 +7014,7 @@
       <c r="Z50" t="inlineStr"/>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB50" t="n">
@@ -7117,7 +7117,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U51" t="inlineStr">
@@ -7146,7 +7146,7 @@
       <c r="Z51" t="inlineStr"/>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB51" t="n">
@@ -7249,7 +7249,7 @@
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U52" t="inlineStr">
@@ -7278,7 +7278,7 @@
       <c r="Z52" t="inlineStr"/>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB52" t="n">
@@ -7377,7 +7377,7 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U53" t="inlineStr">
@@ -7406,7 +7406,7 @@
       <c r="Z53" t="inlineStr"/>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB53" t="n">
@@ -7505,7 +7505,7 @@
       </c>
       <c r="T54" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U54" t="inlineStr">
@@ -7534,7 +7534,7 @@
       <c r="Z54" t="inlineStr"/>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB54" t="n">
@@ -7637,7 +7637,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U55" t="inlineStr">
@@ -7666,7 +7666,7 @@
       <c r="Z55" t="inlineStr"/>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB55" t="n">
@@ -7765,7 +7765,7 @@
       </c>
       <c r="T56" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U56" t="inlineStr">
@@ -7794,7 +7794,7 @@
       <c r="Z56" t="inlineStr"/>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB56" t="n">
@@ -7897,7 +7897,7 @@
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U57" t="inlineStr">
@@ -7926,7 +7926,7 @@
       <c r="Z57" t="inlineStr"/>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB57" t="n">
@@ -8029,7 +8029,7 @@
       </c>
       <c r="T58" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U58" t="inlineStr">
@@ -8058,7 +8058,7 @@
       <c r="Z58" t="inlineStr"/>
       <c r="AA58" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB58" t="n">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="T59" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U59" t="inlineStr">
@@ -8190,7 +8190,7 @@
       <c r="Z59" t="inlineStr"/>
       <c r="AA59" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB59" t="n">
@@ -8322,7 +8322,7 @@
       <c r="Z60" t="inlineStr"/>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB60" t="n">
@@ -8454,7 +8454,7 @@
       <c r="Z61" t="inlineStr"/>
       <c r="AA61" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB61" t="n">
@@ -8557,7 +8557,7 @@
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U62" t="inlineStr">
@@ -8586,7 +8586,7 @@
       <c r="Z62" t="inlineStr"/>
       <c r="AA62" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB62" t="n">
@@ -8689,7 +8689,7 @@
       </c>
       <c r="T63" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U63" t="inlineStr">
@@ -8718,7 +8718,7 @@
       <c r="Z63" t="inlineStr"/>
       <c r="AA63" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB63" t="n">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="T64" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U64" t="inlineStr">
@@ -8850,7 +8850,7 @@
       <c r="Z64" t="inlineStr"/>
       <c r="AA64" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB64" t="n">
@@ -8953,7 +8953,7 @@
       </c>
       <c r="T65" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U65" t="inlineStr">
@@ -8982,7 +8982,7 @@
       <c r="Z65" t="inlineStr"/>
       <c r="AA65" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB65" t="n">
@@ -9085,7 +9085,7 @@
       </c>
       <c r="T66" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
@@ -9114,7 +9114,7 @@
       <c r="Z66" t="inlineStr"/>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB66" t="n">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="T67" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U67" t="inlineStr">
@@ -9242,7 +9242,7 @@
       <c r="Z67" t="inlineStr"/>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB67" t="n">
@@ -9345,7 +9345,7 @@
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
@@ -9374,7 +9374,7 @@
       <c r="Z68" t="inlineStr"/>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB68" t="n">
@@ -9477,7 +9477,7 @@
       </c>
       <c r="T69" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
@@ -9506,7 +9506,7 @@
       <c r="Z69" t="inlineStr"/>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB69" t="n">
@@ -9609,7 +9609,7 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U70" t="inlineStr">
@@ -9638,7 +9638,7 @@
       <c r="Z70" t="inlineStr"/>
       <c r="AA70" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB70" t="n">
@@ -9741,7 +9741,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U71" t="inlineStr">
@@ -9770,7 +9770,7 @@
       <c r="Z71" t="inlineStr"/>
       <c r="AA71" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB71" t="n">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U72" t="inlineStr">
@@ -9898,7 +9898,7 @@
       <c r="Z72" t="inlineStr"/>
       <c r="AA72" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB72" t="n">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U73" t="inlineStr">
@@ -10030,7 +10030,7 @@
       <c r="Z73" t="inlineStr"/>
       <c r="AA73" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB73" t="n">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="T74" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U74" t="inlineStr">
@@ -10162,7 +10162,7 @@
       <c r="Z74" t="inlineStr"/>
       <c r="AA74" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB74" t="n">
@@ -10261,7 +10261,7 @@
       </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U75" t="inlineStr">
@@ -10290,7 +10290,7 @@
       <c r="Z75" t="inlineStr"/>
       <c r="AA75" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB75" t="n">
@@ -10393,7 +10393,7 @@
       </c>
       <c r="T76" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U76" t="inlineStr">
@@ -10422,7 +10422,7 @@
       <c r="Z76" t="inlineStr"/>
       <c r="AA76" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB76" t="n">
@@ -10525,7 +10525,7 @@
       </c>
       <c r="T77" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
@@ -10554,7 +10554,7 @@
       <c r="Z77" t="inlineStr"/>
       <c r="AA77" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB77" t="n">
@@ -10657,7 +10657,7 @@
       </c>
       <c r="T78" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U78" t="inlineStr">
@@ -10686,7 +10686,7 @@
       <c r="Z78" t="inlineStr"/>
       <c r="AA78" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB78" t="n">
@@ -10789,7 +10789,7 @@
       </c>
       <c r="T79" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U79" t="inlineStr">
@@ -10818,7 +10818,7 @@
       <c r="Z79" t="inlineStr"/>
       <c r="AA79" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB79" t="n">
@@ -10921,7 +10921,7 @@
       </c>
       <c r="T80" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U80" t="inlineStr">
@@ -10950,7 +10950,7 @@
       <c r="Z80" t="inlineStr"/>
       <c r="AA80" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB80" t="n">
@@ -11053,7 +11053,7 @@
       </c>
       <c r="T81" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U81" t="inlineStr">
@@ -11082,7 +11082,7 @@
       <c r="Z81" t="inlineStr"/>
       <c r="AA81" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB81" t="n">
@@ -11181,7 +11181,7 @@
       </c>
       <c r="T82" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U82" t="inlineStr">
@@ -11210,7 +11210,7 @@
       <c r="Z82" t="inlineStr"/>
       <c r="AA82" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB82" t="n">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="T83" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U83" t="inlineStr">
@@ -11342,7 +11342,7 @@
       <c r="Z83" t="inlineStr"/>
       <c r="AA83" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB83" t="n">
@@ -11445,7 +11445,7 @@
       </c>
       <c r="T84" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U84" t="inlineStr">
@@ -11474,7 +11474,7 @@
       <c r="Z84" t="inlineStr"/>
       <c r="AA84" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB84" t="n">
@@ -11577,7 +11577,7 @@
       </c>
       <c r="T85" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U85" t="inlineStr">
@@ -11606,7 +11606,7 @@
       <c r="Z85" t="inlineStr"/>
       <c r="AA85" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB85" t="n">
@@ -11705,7 +11705,7 @@
       </c>
       <c r="T86" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U86" t="inlineStr">
@@ -11734,7 +11734,7 @@
       <c r="Z86" t="inlineStr"/>
       <c r="AA86" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB86" t="n">
@@ -11837,7 +11837,7 @@
       </c>
       <c r="T87" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U87" t="inlineStr">
@@ -11866,7 +11866,7 @@
       <c r="Z87" t="inlineStr"/>
       <c r="AA87" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB87" t="n">
@@ -11965,7 +11965,7 @@
       </c>
       <c r="T88" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U88" t="inlineStr">
@@ -11994,7 +11994,7 @@
       <c r="Z88" t="inlineStr"/>
       <c r="AA88" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB88" t="n">
@@ -12097,7 +12097,7 @@
       </c>
       <c r="T89" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U89" t="inlineStr">
@@ -12126,7 +12126,7 @@
       <c r="Z89" t="inlineStr"/>
       <c r="AA89" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB89" t="n">
@@ -12225,7 +12225,7 @@
       </c>
       <c r="T90" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U90" t="inlineStr">
@@ -12254,7 +12254,7 @@
       <c r="Z90" t="inlineStr"/>
       <c r="AA90" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB90" t="n">
@@ -12357,7 +12357,7 @@
       </c>
       <c r="T91" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U91" t="inlineStr">
@@ -12386,7 +12386,7 @@
       <c r="Z91" t="inlineStr"/>
       <c r="AA91" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB91" t="n">
@@ -12485,7 +12485,7 @@
       </c>
       <c r="T92" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U92" t="inlineStr">
@@ -12514,7 +12514,7 @@
       <c r="Z92" t="inlineStr"/>
       <c r="AA92" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB92" t="n">
@@ -12613,7 +12613,7 @@
       </c>
       <c r="T93" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U93" t="inlineStr">
@@ -12642,7 +12642,7 @@
       <c r="Z93" t="inlineStr"/>
       <c r="AA93" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB93" t="n">
@@ -12745,7 +12745,7 @@
       </c>
       <c r="T94" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U94" t="inlineStr">
@@ -12774,7 +12774,7 @@
       <c r="Z94" t="inlineStr"/>
       <c r="AA94" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB94" t="n">
@@ -12877,7 +12877,7 @@
       </c>
       <c r="T95" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U95" t="inlineStr">
@@ -12906,7 +12906,7 @@
       <c r="Z95" t="inlineStr"/>
       <c r="AA95" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB95" t="n">
@@ -13009,7 +13009,7 @@
       </c>
       <c r="T96" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U96" t="inlineStr">
@@ -13038,7 +13038,7 @@
       <c r="Z96" t="inlineStr"/>
       <c r="AA96" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB96" t="n">
@@ -13141,7 +13141,7 @@
       </c>
       <c r="T97" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U97" t="inlineStr">
@@ -13170,7 +13170,7 @@
       <c r="Z97" t="inlineStr"/>
       <c r="AA97" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB97" t="n">
@@ -13273,7 +13273,7 @@
       </c>
       <c r="T98" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U98" t="inlineStr">
@@ -13302,7 +13302,7 @@
       <c r="Z98" t="inlineStr"/>
       <c r="AA98" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB98" t="n">
@@ -13405,7 +13405,7 @@
       </c>
       <c r="T99" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U99" t="inlineStr">
@@ -13434,7 +13434,7 @@
       <c r="Z99" t="inlineStr"/>
       <c r="AA99" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB99" t="n">
@@ -13537,7 +13537,7 @@
       </c>
       <c r="T100" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U100" t="inlineStr">
@@ -13566,7 +13566,7 @@
       <c r="Z100" t="inlineStr"/>
       <c r="AA100" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB100" t="n">
@@ -13669,7 +13669,7 @@
       </c>
       <c r="T101" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U101" t="inlineStr">
@@ -13698,7 +13698,7 @@
       <c r="Z101" t="inlineStr"/>
       <c r="AA101" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB101" t="n">
@@ -13801,7 +13801,7 @@
       </c>
       <c r="T102" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U102" t="inlineStr">
@@ -13830,7 +13830,7 @@
       <c r="Z102" t="inlineStr"/>
       <c r="AA102" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB102" t="n">
@@ -13933,7 +13933,7 @@
       </c>
       <c r="T103" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U103" t="inlineStr">
@@ -13962,7 +13962,7 @@
       <c r="Z103" t="inlineStr"/>
       <c r="AA103" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB103" t="n">
@@ -14065,7 +14065,7 @@
       </c>
       <c r="T104" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U104" t="inlineStr">
@@ -14094,7 +14094,7 @@
       <c r="Z104" t="inlineStr"/>
       <c r="AA104" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB104" t="n">
@@ -14197,7 +14197,7 @@
       </c>
       <c r="T105" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U105" t="inlineStr">
@@ -14226,7 +14226,7 @@
       <c r="Z105" t="inlineStr"/>
       <c r="AA105" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB105" t="n">
@@ -14329,7 +14329,7 @@
       </c>
       <c r="T106" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U106" t="inlineStr">
@@ -14358,7 +14358,7 @@
       <c r="Z106" t="inlineStr"/>
       <c r="AA106" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB106" t="n">
@@ -14461,7 +14461,7 @@
       </c>
       <c r="T107" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U107" t="inlineStr">
@@ -14490,7 +14490,7 @@
       <c r="Z107" t="inlineStr"/>
       <c r="AA107" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB107" t="n">
@@ -14593,7 +14593,7 @@
       </c>
       <c r="T108" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U108" t="inlineStr">
@@ -14622,7 +14622,7 @@
       <c r="Z108" t="inlineStr"/>
       <c r="AA108" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB108" t="n">
@@ -14725,7 +14725,7 @@
       </c>
       <c r="T109" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U109" t="inlineStr">
@@ -14754,7 +14754,7 @@
       <c r="Z109" t="inlineStr"/>
       <c r="AA109" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB109" t="n">
@@ -14853,7 +14853,7 @@
       </c>
       <c r="T110" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U110" t="inlineStr">
@@ -14882,7 +14882,7 @@
       <c r="Z110" t="inlineStr"/>
       <c r="AA110" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB110" t="n">
@@ -14985,7 +14985,7 @@
       </c>
       <c r="T111" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U111" t="inlineStr">
@@ -15014,7 +15014,7 @@
       <c r="Z111" t="inlineStr"/>
       <c r="AA111" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB111" t="n">
@@ -15117,7 +15117,7 @@
       </c>
       <c r="T112" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U112" t="inlineStr">
@@ -15146,7 +15146,7 @@
       <c r="Z112" t="inlineStr"/>
       <c r="AA112" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB112" t="n">
@@ -15249,7 +15249,7 @@
       </c>
       <c r="T113" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U113" t="inlineStr">
@@ -15278,7 +15278,7 @@
       <c r="Z113" t="inlineStr"/>
       <c r="AA113" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB113" t="n">
@@ -15381,7 +15381,7 @@
       </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U114" t="inlineStr">
@@ -15410,7 +15410,7 @@
       <c r="Z114" t="inlineStr"/>
       <c r="AA114" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB114" t="n">
@@ -15513,7 +15513,7 @@
       </c>
       <c r="T115" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U115" t="inlineStr">
@@ -15542,7 +15542,7 @@
       <c r="Z115" t="inlineStr"/>
       <c r="AA115" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB115" t="n">
@@ -15670,7 +15670,7 @@
       <c r="Z116" t="inlineStr"/>
       <c r="AA116" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB116" t="n">
@@ -15773,7 +15773,7 @@
       </c>
       <c r="T117" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U117" t="inlineStr">
@@ -15802,7 +15802,7 @@
       <c r="Z117" t="inlineStr"/>
       <c r="AA117" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB117" t="n">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="T118" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U118" t="inlineStr">
@@ -15934,7 +15934,7 @@
       <c r="Z118" t="inlineStr"/>
       <c r="AA118" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB118" t="n">
@@ -16037,7 +16037,7 @@
       </c>
       <c r="T119" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U119" t="inlineStr">
@@ -16066,7 +16066,7 @@
       <c r="Z119" t="inlineStr"/>
       <c r="AA119" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB119" t="n">
@@ -16169,7 +16169,7 @@
       </c>
       <c r="T120" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U120" t="inlineStr">
@@ -16198,7 +16198,7 @@
       <c r="Z120" t="inlineStr"/>
       <c r="AA120" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB120" t="n">
@@ -16301,7 +16301,7 @@
       </c>
       <c r="T121" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U121" t="inlineStr">
@@ -16330,7 +16330,7 @@
       <c r="Z121" t="inlineStr"/>
       <c r="AA121" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB121" t="n">
@@ -16433,7 +16433,7 @@
       </c>
       <c r="T122" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U122" t="inlineStr">
@@ -16462,7 +16462,7 @@
       <c r="Z122" t="inlineStr"/>
       <c r="AA122" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB122" t="n">
@@ -16565,7 +16565,7 @@
       </c>
       <c r="T123" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U123" t="inlineStr">
@@ -16594,7 +16594,7 @@
       <c r="Z123" t="inlineStr"/>
       <c r="AA123" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB123" t="n">
@@ -16697,7 +16697,7 @@
       </c>
       <c r="T124" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U124" t="inlineStr">
@@ -16726,7 +16726,7 @@
       <c r="Z124" t="inlineStr"/>
       <c r="AA124" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB124" t="n">
@@ -16829,7 +16829,7 @@
       </c>
       <c r="T125" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U125" t="inlineStr">
@@ -16858,7 +16858,7 @@
       <c r="Z125" t="inlineStr"/>
       <c r="AA125" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB125" t="n">
@@ -16961,7 +16961,7 @@
       </c>
       <c r="T126" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U126" t="inlineStr">
@@ -16990,7 +16990,7 @@
       <c r="Z126" t="inlineStr"/>
       <c r="AA126" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB126" t="n">
@@ -17093,7 +17093,7 @@
       </c>
       <c r="T127" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U127" t="inlineStr">
@@ -17122,7 +17122,7 @@
       <c r="Z127" t="inlineStr"/>
       <c r="AA127" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB127" t="n">
@@ -17225,7 +17225,7 @@
       </c>
       <c r="T128" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U128" t="inlineStr">
@@ -17254,7 +17254,7 @@
       <c r="Z128" t="inlineStr"/>
       <c r="AA128" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB128" t="n">
@@ -17357,7 +17357,7 @@
       </c>
       <c r="T129" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U129" t="inlineStr">
@@ -17386,7 +17386,7 @@
       <c r="Z129" t="inlineStr"/>
       <c r="AA129" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB129" t="n">
@@ -17489,7 +17489,7 @@
       </c>
       <c r="T130" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U130" t="inlineStr">
@@ -17518,7 +17518,7 @@
       <c r="Z130" t="inlineStr"/>
       <c r="AA130" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB130" t="n">
@@ -17621,7 +17621,7 @@
       </c>
       <c r="T131" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U131" t="inlineStr">
@@ -17650,7 +17650,7 @@
       <c r="Z131" t="inlineStr"/>
       <c r="AA131" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB131" t="n">
@@ -17753,7 +17753,7 @@
       </c>
       <c r="T132" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U132" t="inlineStr">
@@ -17782,7 +17782,7 @@
       <c r="Z132" t="inlineStr"/>
       <c r="AA132" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB132" t="n">
@@ -17885,7 +17885,7 @@
       </c>
       <c r="T133" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U133" t="inlineStr">
@@ -17914,7 +17914,7 @@
       <c r="Z133" t="inlineStr"/>
       <c r="AA133" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB133" t="n">
@@ -18017,7 +18017,7 @@
       </c>
       <c r="T134" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U134" t="inlineStr">
@@ -18046,7 +18046,7 @@
       <c r="Z134" t="inlineStr"/>
       <c r="AA134" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB134" t="n">
@@ -18149,7 +18149,7 @@
       </c>
       <c r="T135" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U135" t="inlineStr">
@@ -18178,7 +18178,7 @@
       <c r="Z135" t="inlineStr"/>
       <c r="AA135" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB135" t="n">
@@ -18277,7 +18277,7 @@
       </c>
       <c r="T136" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U136" t="inlineStr">
@@ -18306,7 +18306,7 @@
       <c r="Z136" t="inlineStr"/>
       <c r="AA136" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB136" t="n">
@@ -18409,7 +18409,7 @@
       </c>
       <c r="T137" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U137" t="inlineStr">
@@ -18438,7 +18438,7 @@
       <c r="Z137" t="inlineStr"/>
       <c r="AA137" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB137" t="n">
@@ -18541,7 +18541,7 @@
       </c>
       <c r="T138" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U138" t="inlineStr">
@@ -18570,7 +18570,7 @@
       <c r="Z138" t="inlineStr"/>
       <c r="AA138" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB138" t="n">
@@ -18702,7 +18702,7 @@
       <c r="Z139" t="inlineStr"/>
       <c r="AA139" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB139" t="n">
@@ -18801,7 +18801,7 @@
       </c>
       <c r="T140" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U140" t="inlineStr">
@@ -18830,7 +18830,7 @@
       <c r="Z140" t="inlineStr"/>
       <c r="AA140" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB140" t="n">
@@ -18933,7 +18933,7 @@
       </c>
       <c r="T141" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U141" t="inlineStr">
@@ -18962,7 +18962,7 @@
       <c r="Z141" t="inlineStr"/>
       <c r="AA141" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB141" t="n">
@@ -19065,7 +19065,7 @@
       </c>
       <c r="T142" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U142" t="inlineStr">
@@ -19094,7 +19094,7 @@
       <c r="Z142" t="inlineStr"/>
       <c r="AA142" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB142" t="n">
@@ -19193,7 +19193,7 @@
       </c>
       <c r="T143" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U143" t="inlineStr">
@@ -19222,7 +19222,7 @@
       <c r="Z143" t="inlineStr"/>
       <c r="AA143" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB143" t="n">
@@ -19354,7 +19354,7 @@
       <c r="Z144" t="inlineStr"/>
       <c r="AA144" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB144" t="n">
@@ -19457,7 +19457,7 @@
       </c>
       <c r="T145" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U145" t="inlineStr">
@@ -19486,7 +19486,7 @@
       <c r="Z145" t="inlineStr"/>
       <c r="AA145" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB145" t="n">
@@ -19589,7 +19589,7 @@
       </c>
       <c r="T146" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U146" t="inlineStr">
@@ -19618,7 +19618,7 @@
       <c r="Z146" t="inlineStr"/>
       <c r="AA146" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB146" t="n">
@@ -19721,7 +19721,7 @@
       </c>
       <c r="T147" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U147" t="inlineStr">
@@ -19750,7 +19750,7 @@
       <c r="Z147" t="inlineStr"/>
       <c r="AA147" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB147" t="n">
@@ -19853,7 +19853,7 @@
       </c>
       <c r="T148" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U148" t="inlineStr">
@@ -19882,7 +19882,7 @@
       <c r="Z148" t="inlineStr"/>
       <c r="AA148" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB148" t="n">
@@ -19985,7 +19985,7 @@
       </c>
       <c r="T149" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U149" t="inlineStr">
@@ -20014,7 +20014,7 @@
       <c r="Z149" t="inlineStr"/>
       <c r="AA149" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB149" t="n">
@@ -20117,7 +20117,7 @@
       </c>
       <c r="T150" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U150" t="inlineStr">
@@ -20146,7 +20146,7 @@
       <c r="Z150" t="inlineStr"/>
       <c r="AA150" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB150" t="n">
@@ -20249,7 +20249,7 @@
       </c>
       <c r="T151" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U151" t="inlineStr">
@@ -20278,7 +20278,7 @@
       <c r="Z151" t="inlineStr"/>
       <c r="AA151" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB151" t="n">
@@ -20381,7 +20381,7 @@
       </c>
       <c r="T152" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U152" t="inlineStr">
@@ -20410,7 +20410,7 @@
       <c r="Z152" t="inlineStr"/>
       <c r="AA152" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB152" t="n">
@@ -20509,7 +20509,7 @@
       </c>
       <c r="T153" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U153" t="inlineStr">
@@ -20538,7 +20538,7 @@
       <c r="Z153" t="inlineStr"/>
       <c r="AA153" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB153" t="n">
@@ -20641,7 +20641,7 @@
       </c>
       <c r="T154" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U154" t="inlineStr">
@@ -20670,7 +20670,7 @@
       <c r="Z154" t="inlineStr"/>
       <c r="AA154" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB154" t="n">
@@ -20773,7 +20773,7 @@
       </c>
       <c r="T155" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U155" t="inlineStr">
@@ -20802,7 +20802,7 @@
       <c r="Z155" t="inlineStr"/>
       <c r="AA155" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB155" t="n">
@@ -20905,7 +20905,7 @@
       </c>
       <c r="T156" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U156" t="inlineStr">
@@ -20934,7 +20934,7 @@
       <c r="Z156" t="inlineStr"/>
       <c r="AA156" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB156" t="n">
@@ -21037,7 +21037,7 @@
       </c>
       <c r="T157" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U157" t="inlineStr">
@@ -21066,7 +21066,7 @@
       <c r="Z157" t="inlineStr"/>
       <c r="AA157" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB157" t="n">
@@ -21169,7 +21169,7 @@
       </c>
       <c r="T158" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U158" t="inlineStr">
@@ -21198,7 +21198,7 @@
       <c r="Z158" t="inlineStr"/>
       <c r="AA158" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB158" t="n">
@@ -21301,7 +21301,7 @@
       </c>
       <c r="T159" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U159" t="inlineStr">
@@ -21330,7 +21330,7 @@
       <c r="Z159" t="inlineStr"/>
       <c r="AA159" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB159" t="n">
@@ -21462,7 +21462,7 @@
       <c r="Z160" t="inlineStr"/>
       <c r="AA160" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB160" t="n">
@@ -21565,7 +21565,7 @@
       </c>
       <c r="T161" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U161" t="inlineStr">
@@ -21594,7 +21594,7 @@
       <c r="Z161" t="inlineStr"/>
       <c r="AA161" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB161" t="n">
@@ -21693,7 +21693,7 @@
       </c>
       <c r="T162" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U162" t="inlineStr">
@@ -21722,7 +21722,7 @@
       <c r="Z162" t="inlineStr"/>
       <c r="AA162" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB162" t="n">
@@ -21825,7 +21825,7 @@
       </c>
       <c r="T163" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U163" t="inlineStr">
@@ -21854,7 +21854,7 @@
       <c r="Z163" t="inlineStr"/>
       <c r="AA163" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB163" t="n">
@@ -21953,7 +21953,7 @@
       </c>
       <c r="T164" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U164" t="inlineStr">
@@ -21982,7 +21982,7 @@
       <c r="Z164" t="inlineStr"/>
       <c r="AA164" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB164" t="n">
@@ -22081,7 +22081,7 @@
       </c>
       <c r="T165" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U165" t="inlineStr">
@@ -22110,7 +22110,7 @@
       <c r="Z165" t="inlineStr"/>
       <c r="AA165" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB165" t="n">
@@ -22213,7 +22213,7 @@
       </c>
       <c r="T166" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U166" t="inlineStr">
@@ -22242,7 +22242,7 @@
       <c r="Z166" t="inlineStr"/>
       <c r="AA166" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB166" t="n">
@@ -22345,7 +22345,7 @@
       </c>
       <c r="T167" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U167" t="inlineStr">
@@ -22374,7 +22374,7 @@
       <c r="Z167" t="inlineStr"/>
       <c r="AA167" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB167" t="n">
@@ -22477,7 +22477,7 @@
       </c>
       <c r="T168" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U168" t="inlineStr">
@@ -22506,7 +22506,7 @@
       <c r="Z168" t="inlineStr"/>
       <c r="AA168" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB168" t="n">
@@ -22609,7 +22609,7 @@
       </c>
       <c r="T169" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U169" t="inlineStr">
@@ -22638,7 +22638,7 @@
       <c r="Z169" t="inlineStr"/>
       <c r="AA169" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB169" t="n">
@@ -22741,7 +22741,7 @@
       </c>
       <c r="T170" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U170" t="inlineStr">
@@ -22770,7 +22770,7 @@
       <c r="Z170" t="inlineStr"/>
       <c r="AA170" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB170" t="n">
@@ -22873,7 +22873,7 @@
       </c>
       <c r="T171" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U171" t="inlineStr">
@@ -22902,7 +22902,7 @@
       <c r="Z171" t="inlineStr"/>
       <c r="AA171" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB171" t="n">
@@ -23030,7 +23030,7 @@
       <c r="Z172" t="inlineStr"/>
       <c r="AA172" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB172" t="n">
@@ -23133,7 +23133,7 @@
       </c>
       <c r="T173" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U173" t="inlineStr">
@@ -23162,7 +23162,7 @@
       <c r="Z173" t="inlineStr"/>
       <c r="AA173" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB173" t="n">
@@ -23265,7 +23265,7 @@
       </c>
       <c r="T174" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U174" t="inlineStr">
@@ -23294,7 +23294,7 @@
       <c r="Z174" t="inlineStr"/>
       <c r="AA174" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB174" t="n">
@@ -23397,7 +23397,7 @@
       </c>
       <c r="T175" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U175" t="inlineStr">
@@ -23426,7 +23426,7 @@
       <c r="Z175" t="inlineStr"/>
       <c r="AA175" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB175" t="n">
@@ -23558,7 +23558,7 @@
       <c r="Z176" t="inlineStr"/>
       <c r="AA176" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB176" t="n">
@@ -23661,7 +23661,7 @@
       </c>
       <c r="T177" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U177" t="inlineStr">
@@ -23690,7 +23690,7 @@
       <c r="Z177" t="inlineStr"/>
       <c r="AA177" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB177" t="n">
@@ -23793,7 +23793,7 @@
       </c>
       <c r="T178" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U178" t="inlineStr">
@@ -23822,7 +23822,7 @@
       <c r="Z178" t="inlineStr"/>
       <c r="AA178" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB178" t="n">
@@ -23921,7 +23921,7 @@
       </c>
       <c r="T179" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U179" t="inlineStr">
@@ -23950,7 +23950,7 @@
       <c r="Z179" t="inlineStr"/>
       <c r="AA179" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB179" t="n">
@@ -24053,7 +24053,7 @@
       </c>
       <c r="T180" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U180" t="inlineStr">
@@ -24082,7 +24082,7 @@
       <c r="Z180" t="inlineStr"/>
       <c r="AA180" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB180" t="n">
@@ -24214,7 +24214,7 @@
       <c r="Z181" t="inlineStr"/>
       <c r="AA181" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB181" t="n">
@@ -24317,7 +24317,7 @@
       </c>
       <c r="T182" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U182" t="inlineStr">
@@ -24346,7 +24346,7 @@
       <c r="Z182" t="inlineStr"/>
       <c r="AA182" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB182" t="n">
@@ -24449,7 +24449,7 @@
       </c>
       <c r="T183" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U183" t="inlineStr">
@@ -24478,7 +24478,7 @@
       <c r="Z183" t="inlineStr"/>
       <c r="AA183" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB183" t="n">
@@ -24581,7 +24581,7 @@
       </c>
       <c r="T184" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U184" t="inlineStr">
@@ -24610,7 +24610,7 @@
       <c r="Z184" t="inlineStr"/>
       <c r="AA184" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB184" t="n">
@@ -24713,7 +24713,7 @@
       </c>
       <c r="T185" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U185" t="inlineStr">
@@ -24742,7 +24742,7 @@
       <c r="Z185" t="inlineStr"/>
       <c r="AA185" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB185" t="n">
@@ -24845,7 +24845,7 @@
       </c>
       <c r="T186" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U186" t="inlineStr">
@@ -24874,7 +24874,7 @@
       <c r="Z186" t="inlineStr"/>
       <c r="AA186" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB186" t="n">
@@ -24977,7 +24977,7 @@
       </c>
       <c r="T187" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U187" t="inlineStr">
@@ -25006,7 +25006,7 @@
       <c r="Z187" t="inlineStr"/>
       <c r="AA187" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB187" t="n">
@@ -25134,7 +25134,7 @@
       <c r="Z188" t="inlineStr"/>
       <c r="AA188" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB188" t="n">
@@ -25237,7 +25237,7 @@
       </c>
       <c r="T189" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U189" t="inlineStr">
@@ -25266,7 +25266,7 @@
       <c r="Z189" t="inlineStr"/>
       <c r="AA189" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB189" t="n">
@@ -25369,7 +25369,7 @@
       </c>
       <c r="T190" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U190" t="inlineStr">
@@ -25398,7 +25398,7 @@
       <c r="Z190" t="inlineStr"/>
       <c r="AA190" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB190" t="n">
@@ -25501,7 +25501,7 @@
       </c>
       <c r="T191" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U191" t="inlineStr">
@@ -25530,7 +25530,7 @@
       <c r="Z191" t="inlineStr"/>
       <c r="AA191" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB191" t="n">
@@ -25633,7 +25633,7 @@
       </c>
       <c r="T192" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U192" t="inlineStr">
@@ -25662,7 +25662,7 @@
       <c r="Z192" t="inlineStr"/>
       <c r="AA192" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB192" t="n">
@@ -25765,7 +25765,7 @@
       </c>
       <c r="T193" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U193" t="inlineStr">
@@ -25794,7 +25794,7 @@
       <c r="Z193" t="inlineStr"/>
       <c r="AA193" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB193" t="n">
@@ -25897,7 +25897,7 @@
       </c>
       <c r="T194" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U194" t="inlineStr">
@@ -25926,7 +25926,7 @@
       <c r="Z194" t="inlineStr"/>
       <c r="AA194" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB194" t="n">
@@ -26029,7 +26029,7 @@
       </c>
       <c r="T195" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U195" t="inlineStr">
@@ -26058,7 +26058,7 @@
       <c r="Z195" t="inlineStr"/>
       <c r="AA195" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB195" t="n">
@@ -26161,7 +26161,7 @@
       </c>
       <c r="T196" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U196" t="inlineStr">
@@ -26190,7 +26190,7 @@
       <c r="Z196" t="inlineStr"/>
       <c r="AA196" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB196" t="n">
@@ -26289,7 +26289,7 @@
       </c>
       <c r="T197" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U197" t="inlineStr">
@@ -26318,7 +26318,7 @@
       <c r="Z197" t="inlineStr"/>
       <c r="AA197" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB197" t="n">
@@ -26421,7 +26421,7 @@
       </c>
       <c r="T198" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U198" t="inlineStr">
@@ -26450,7 +26450,7 @@
       <c r="Z198" t="inlineStr"/>
       <c r="AA198" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB198" t="n">
@@ -26553,7 +26553,7 @@
       </c>
       <c r="T199" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U199" t="inlineStr">
@@ -26582,7 +26582,7 @@
       <c r="Z199" t="inlineStr"/>
       <c r="AA199" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB199" t="n">
@@ -26685,7 +26685,7 @@
       </c>
       <c r="T200" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U200" t="inlineStr">
@@ -26714,7 +26714,7 @@
       <c r="Z200" t="inlineStr"/>
       <c r="AA200" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB200" t="n">
@@ -26817,7 +26817,7 @@
       </c>
       <c r="T201" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U201" t="inlineStr">
@@ -26846,7 +26846,7 @@
       <c r="Z201" t="inlineStr"/>
       <c r="AA201" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB201" t="n">
@@ -26945,7 +26945,7 @@
       </c>
       <c r="T202" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U202" t="inlineStr">
@@ -26974,7 +26974,7 @@
       <c r="Z202" t="inlineStr"/>
       <c r="AA202" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB202" t="n">
@@ -27073,7 +27073,7 @@
       </c>
       <c r="T203" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U203" t="inlineStr">
@@ -27102,7 +27102,7 @@
       <c r="Z203" t="inlineStr"/>
       <c r="AA203" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB203" t="n">
@@ -27205,7 +27205,7 @@
       </c>
       <c r="T204" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U204" t="inlineStr">
@@ -27234,7 +27234,7 @@
       <c r="Z204" t="inlineStr"/>
       <c r="AA204" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB204" t="n">
@@ -27337,7 +27337,7 @@
       </c>
       <c r="T205" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U205" t="inlineStr">
@@ -27366,7 +27366,7 @@
       <c r="Z205" t="inlineStr"/>
       <c r="AA205" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB205" t="n">
@@ -27469,7 +27469,7 @@
       </c>
       <c r="T206" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U206" t="inlineStr">
@@ -27498,7 +27498,7 @@
       <c r="Z206" t="inlineStr"/>
       <c r="AA206" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB206" t="n">
@@ -27601,7 +27601,7 @@
       </c>
       <c r="T207" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U207" t="inlineStr">
@@ -27630,7 +27630,7 @@
       <c r="Z207" t="inlineStr"/>
       <c r="AA207" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB207" t="n">
@@ -27733,7 +27733,7 @@
       </c>
       <c r="T208" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U208" t="inlineStr">
@@ -27762,7 +27762,7 @@
       <c r="Z208" t="inlineStr"/>
       <c r="AA208" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB208" t="n">
@@ -27865,7 +27865,7 @@
       </c>
       <c r="T209" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U209" t="inlineStr">
@@ -27894,7 +27894,7 @@
       <c r="Z209" t="inlineStr"/>
       <c r="AA209" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB209" t="n">
@@ -27997,7 +27997,7 @@
       </c>
       <c r="T210" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U210" t="inlineStr">
@@ -28026,7 +28026,7 @@
       <c r="Z210" t="inlineStr"/>
       <c r="AA210" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB210" t="n">
@@ -28129,7 +28129,7 @@
       </c>
       <c r="T211" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U211" t="inlineStr">
@@ -28158,7 +28158,7 @@
       <c r="Z211" t="inlineStr"/>
       <c r="AA211" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB211" t="n">
@@ -28290,7 +28290,7 @@
       <c r="Z212" t="inlineStr"/>
       <c r="AA212" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB212" t="n">
@@ -28393,7 +28393,7 @@
       </c>
       <c r="T213" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U213" t="inlineStr">
@@ -28422,7 +28422,7 @@
       <c r="Z213" t="inlineStr"/>
       <c r="AA213" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB213" t="n">
@@ -28525,7 +28525,7 @@
       </c>
       <c r="T214" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U214" t="inlineStr">
@@ -28554,7 +28554,7 @@
       <c r="Z214" t="inlineStr"/>
       <c r="AA214" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB214" t="n">
@@ -28657,7 +28657,7 @@
       </c>
       <c r="T215" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U215" t="inlineStr">
@@ -28686,7 +28686,7 @@
       <c r="Z215" t="inlineStr"/>
       <c r="AA215" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB215" t="n">
@@ -28789,7 +28789,7 @@
       </c>
       <c r="T216" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U216" t="inlineStr">
@@ -28818,7 +28818,7 @@
       <c r="Z216" t="inlineStr"/>
       <c r="AA216" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB216" t="n">
@@ -28921,7 +28921,7 @@
       </c>
       <c r="T217" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U217" t="inlineStr">
@@ -28950,7 +28950,7 @@
       <c r="Z217" t="inlineStr"/>
       <c r="AA217" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB217" t="n">
@@ -29053,7 +29053,7 @@
       </c>
       <c r="T218" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U218" t="inlineStr">
@@ -29082,7 +29082,7 @@
       <c r="Z218" t="inlineStr"/>
       <c r="AA218" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB218" t="n">
@@ -29185,7 +29185,7 @@
       </c>
       <c r="T219" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U219" t="inlineStr">
@@ -29214,7 +29214,7 @@
       <c r="Z219" t="inlineStr"/>
       <c r="AA219" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB219" t="n">
@@ -29317,7 +29317,7 @@
       </c>
       <c r="T220" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U220" t="inlineStr">
@@ -29346,7 +29346,7 @@
       <c r="Z220" t="inlineStr"/>
       <c r="AA220" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB220" t="n">
@@ -29449,7 +29449,7 @@
       </c>
       <c r="T221" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U221" t="inlineStr">
@@ -29478,7 +29478,7 @@
       <c r="Z221" t="inlineStr"/>
       <c r="AA221" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB221" t="n">
@@ -29581,7 +29581,7 @@
       </c>
       <c r="T222" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U222" t="inlineStr">
@@ -29610,7 +29610,7 @@
       <c r="Z222" t="inlineStr"/>
       <c r="AA222" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB222" t="n">
@@ -29713,7 +29713,7 @@
       </c>
       <c r="T223" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U223" t="inlineStr">
@@ -29742,7 +29742,7 @@
       <c r="Z223" t="inlineStr"/>
       <c r="AA223" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB223" t="n">
@@ -29845,7 +29845,7 @@
       </c>
       <c r="T224" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U224" t="inlineStr">
@@ -29874,7 +29874,7 @@
       <c r="Z224" t="inlineStr"/>
       <c r="AA224" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB224" t="n">
@@ -29977,7 +29977,7 @@
       </c>
       <c r="T225" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MERKEZ</t>
         </is>
       </c>
       <c r="U225" t="inlineStr">
@@ -30006,7 +30006,7 @@
       <c r="Z225" t="inlineStr"/>
       <c r="AA225" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB225" t="n">
@@ -30138,7 +30138,7 @@
       <c r="Z226" t="inlineStr"/>
       <c r="AA226" t="inlineStr">
         <is>
-          <t>08/01/2024</t>
+          <t>09/01/2024</t>
         </is>
       </c>
       <c r="AB226" t="n">

</xml_diff>